<commit_message>
Update stock data files
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/High Energy Batteries (India) Ltd.xlsx
+++ b/dumps/Stocks/High Energy Batteries (India) Ltd.xlsx
@@ -712,7 +712,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1005"/>
+  <dimension ref="A1:AP1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" s="62">
       <c r="A5" s="73" t="n">
-        <v>45957</v>
+        <v>45967</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1078,18 +1078,18 @@
         <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>607.4</v>
+        <v>570.45</v>
       </c>
       <c r="F5" t="n">
-        <v>6104.4</v>
+        <v>5733</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CN#252607382790</t>
+          <t>CN#252607785263</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>30.4</v>
+        <v>28.5</v>
       </c>
       <c r="J5">
         <f>Index!$C$2</f>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" s="62">
       <c r="A6" s="73" t="n">
-        <v>46063</v>
+        <v>45961</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1111,24 +1111,21 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>589.75</v>
+        <v>596.15</v>
       </c>
       <c r="F6" t="n">
-        <v>5946.05</v>
+        <v>2995.65</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>CN#252611730667</t>
+          <t>CN#252607606298</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>5.89</v>
-      </c>
       <c r="I6" t="n">
-        <v>42.66</v>
+        <v>14.9</v>
       </c>
       <c r="J6">
         <f>Index!$C$2</f>
@@ -1136,8 +1133,8 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="62">
-      <c r="A7" s="60" t="n">
-        <v>46050</v>
+      <c r="A7" s="73" t="n">
+        <v>45957</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1153,26 +1150,27 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>530</v>
+        <v>607.4</v>
       </c>
       <c r="F7" t="n">
-        <v>5343.69</v>
+        <v>6104.4</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>CN#252607382790</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>5.33</v>
-      </c>
       <c r="I7" t="n">
-        <v>38.36</v>
+        <v>30.4</v>
+      </c>
+      <c r="J7">
+        <f>Index!$C$2</f>
+        <v/>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="62">
-      <c r="A8" s="60" t="n">
-        <v>46049</v>
+      <c r="A8" s="73" t="n">
+        <v>46063</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1185,29 +1183,33 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>534.7</v>
+        <v>589.75</v>
       </c>
       <c r="F8" t="n">
-        <v>2695.48</v>
+        <v>5946.05</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>CN#252611730667</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>2.67</v>
+        <v>5.89</v>
       </c>
       <c r="I8" t="n">
-        <v>19.31</v>
+        <v>42.66</v>
+      </c>
+      <c r="J8">
+        <f>Index!$C$2</f>
+        <v/>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="62">
       <c r="A9" s="60" t="n">
-        <v>46042</v>
+        <v>46050</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1223,10 +1225,10 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="F9" t="n">
-        <v>5454.64</v>
+        <v>5343.69</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -1234,15 +1236,15 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>5.42</v>
+        <v>5.33</v>
       </c>
       <c r="I9" t="n">
-        <v>39.22</v>
+        <v>38.36</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="62">
       <c r="A10" s="60" t="n">
-        <v>46030</v>
+        <v>46049</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1255,13 +1257,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E10" t="n">
-        <v>563.85</v>
+        <v>534.7</v>
       </c>
       <c r="F10" t="n">
-        <v>5684.91</v>
+        <v>2695.48</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1269,15 +1271,15 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>5.62</v>
+        <v>2.67</v>
       </c>
       <c r="I10" t="n">
-        <v>40.79</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="62">
       <c r="A11" s="60" t="n">
-        <v>46017</v>
+        <v>46042</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1290,13 +1292,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>545.55</v>
+        <v>541</v>
       </c>
       <c r="F11" t="n">
-        <v>2750.24</v>
+        <v>5454.64</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1304,15 +1306,15 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>2.74</v>
+        <v>5.42</v>
       </c>
       <c r="I11" t="n">
-        <v>19.75</v>
+        <v>39.22</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="62">
       <c r="A12" s="60" t="n">
-        <v>46017</v>
+        <v>46030</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1325,13 +1327,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>545.5</v>
+        <v>563.85</v>
       </c>
       <c r="F12" t="n">
-        <v>2749.99</v>
+        <v>5684.91</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1339,15 +1341,15 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>2.74</v>
+        <v>5.62</v>
       </c>
       <c r="I12" t="n">
-        <v>19.75</v>
+        <v>40.79</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="62">
       <c r="A13" s="60" t="n">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1360,13 +1362,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>545.25</v>
+        <v>545.55</v>
       </c>
       <c r="F13" t="n">
-        <v>5497.42</v>
+        <v>2750.24</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1374,15 +1376,15 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>5.42</v>
+        <v>2.74</v>
       </c>
       <c r="I13" t="n">
-        <v>39.5</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="62">
       <c r="A14" s="60" t="n">
-        <v>46014</v>
+        <v>46017</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1395,13 +1397,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>548.9</v>
+        <v>545.5</v>
       </c>
       <c r="F14" t="n">
-        <v>5534.11</v>
+        <v>2749.99</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1409,15 +1411,15 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>5.47</v>
+        <v>2.74</v>
       </c>
       <c r="I14" t="n">
-        <v>39.64</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="62">
       <c r="A15" s="60" t="n">
-        <v>46007</v>
+        <v>46015</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1433,10 +1435,10 @@
         <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>541.3</v>
+        <v>545.25</v>
       </c>
       <c r="F15" t="n">
-        <v>5457.59</v>
+        <v>5497.42</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1444,15 +1446,15 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>5.39</v>
+        <v>5.42</v>
       </c>
       <c r="I15" t="n">
-        <v>39.2</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="62">
       <c r="A16" s="60" t="n">
-        <v>46002</v>
+        <v>46014</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1465,13 +1467,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>547.9</v>
+        <v>548.9</v>
       </c>
       <c r="F16" t="n">
-        <v>2762.01</v>
+        <v>5534.11</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1479,15 +1481,15 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>2.75</v>
+        <v>5.47</v>
       </c>
       <c r="I16" t="n">
-        <v>19.76</v>
+        <v>39.64</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="62">
       <c r="A17" s="60" t="n">
-        <v>46000</v>
+        <v>46007</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1500,13 +1502,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>560.95</v>
+        <v>541.3</v>
       </c>
       <c r="F17" t="n">
-        <v>2827.8</v>
+        <v>5457.59</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1514,15 +1516,15 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>2.8</v>
+        <v>5.39</v>
       </c>
       <c r="I17" t="n">
-        <v>20.25</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="62">
       <c r="A18" s="60" t="n">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1538,10 +1540,10 @@
         <v>5</v>
       </c>
       <c r="E18" t="n">
-        <v>561</v>
+        <v>547.9</v>
       </c>
       <c r="F18" t="n">
-        <v>2828.11</v>
+        <v>2762.01</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1549,15 +1551,15 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>2.8</v>
+        <v>2.75</v>
       </c>
       <c r="I18" t="n">
-        <v>20.31</v>
+        <v>19.76</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="62">
       <c r="A19" s="60" t="n">
-        <v>45996</v>
+        <v>46000</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1570,13 +1572,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>573.95</v>
+        <v>560.95</v>
       </c>
       <c r="F19" t="n">
-        <v>5786.76</v>
+        <v>2827.8</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1584,15 +1586,15 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>5.72</v>
+        <v>2.8</v>
       </c>
       <c r="I19" t="n">
-        <v>41.54</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="62">
       <c r="A20" s="60" t="n">
-        <v>45989</v>
+        <v>46000</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1608,10 +1610,10 @@
         <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>586.95</v>
+        <v>561</v>
       </c>
       <c r="F20" t="n">
-        <v>2958.88</v>
+        <v>2828.11</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1619,15 +1621,15 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>2.93</v>
+        <v>2.8</v>
       </c>
       <c r="I20" t="n">
-        <v>21.2</v>
+        <v>20.31</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="62">
       <c r="A21" s="60" t="n">
-        <v>45982</v>
+        <v>45996</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1640,13 +1642,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>621</v>
+        <v>573.95</v>
       </c>
       <c r="F21" t="n">
-        <v>3130.59</v>
+        <v>5786.76</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1654,15 +1656,15 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>3.11</v>
+        <v>5.72</v>
       </c>
       <c r="I21" t="n">
-        <v>22.48</v>
+        <v>41.54</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="62">
       <c r="A22" s="60" t="n">
-        <v>45979</v>
+        <v>45989</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1675,13 +1677,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>624.95</v>
+        <v>586.95</v>
       </c>
       <c r="F22" t="n">
-        <v>1260.17</v>
+        <v>2958.88</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1689,15 +1691,15 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>1.25</v>
+        <v>2.93</v>
       </c>
       <c r="I22" t="n">
-        <v>9.02</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="62">
       <c r="A23" s="60" t="n">
-        <v>45979</v>
+        <v>45982</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1710,13 +1712,13 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>622.8</v>
+        <v>621</v>
       </c>
       <c r="F23" t="n">
-        <v>1883.78</v>
+        <v>3130.59</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1724,15 +1726,15 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>1.88</v>
+        <v>3.11</v>
       </c>
       <c r="I23" t="n">
-        <v>13.5</v>
+        <v>22.48</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="62">
       <c r="A24" s="60" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1745,13 +1747,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="n">
-        <v>658</v>
+        <v>624.95</v>
       </c>
       <c r="F24" t="n">
-        <v>663.4299999999999</v>
+        <v>1260.17</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1759,15 +1761,15 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>0.66</v>
+        <v>1.25</v>
       </c>
       <c r="I24" t="n">
-        <v>4.77</v>
+        <v>9.02</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="62">
       <c r="A25" s="60" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1780,13 +1782,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" t="n">
-        <v>657.95</v>
+        <v>622.8</v>
       </c>
       <c r="F25" t="n">
-        <v>1326.73</v>
+        <v>1883.78</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1794,10 +1796,10 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>1.32</v>
+        <v>1.88</v>
       </c>
       <c r="I25" t="n">
-        <v>9.51</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="62">
@@ -1815,13 +1817,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F26" t="n">
-        <v>1324.82</v>
+        <v>663.4299999999999</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1829,15 +1831,15 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>1.32</v>
+        <v>0.66</v>
       </c>
       <c r="I26" t="n">
-        <v>9.5</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="62">
       <c r="A27" s="60" t="n">
-        <v>45967</v>
+        <v>45978</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1850,13 +1852,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E27" t="n">
-        <v>570.45</v>
+        <v>657.95</v>
       </c>
       <c r="F27" t="n">
-        <v>5751.49</v>
+        <v>1326.73</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1864,15 +1866,15 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>5.74</v>
+        <v>1.32</v>
       </c>
       <c r="I27" t="n">
-        <v>41.25</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="62">
       <c r="A28" s="60" t="n">
-        <v>45961</v>
+        <v>45978</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1885,13 +1887,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>596.15</v>
+        <v>657</v>
       </c>
       <c r="F28" t="n">
-        <v>3005.27</v>
+        <v>1324.82</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1899,15 +1901,15 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>2.97</v>
+        <v>1.32</v>
       </c>
       <c r="I28" t="n">
-        <v>21.55</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="62">
       <c r="A29" s="60" t="n">
-        <v>45957</v>
+        <v>45967</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1923,10 +1925,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="n">
-        <v>607.4</v>
+        <v>570.45</v>
       </c>
       <c r="F29" t="n">
-        <v>6124.02</v>
+        <v>5751.49</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1934,15 +1936,15 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>6.08</v>
+        <v>5.74</v>
       </c>
       <c r="I29" t="n">
-        <v>43.94</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="62">
       <c r="A30" s="60" t="n">
-        <v>45954</v>
+        <v>45961</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1958,10 +1960,10 @@
         <v>5</v>
       </c>
       <c r="E30" t="n">
-        <v>647.9</v>
+        <v>596.15</v>
       </c>
       <c r="F30" t="n">
-        <v>3266.17</v>
+        <v>3005.27</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1969,15 +1971,15 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>3.24</v>
+        <v>2.97</v>
       </c>
       <c r="I30" t="n">
-        <v>23.43</v>
+        <v>21.55</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="62">
       <c r="A31" s="60" t="n">
-        <v>45953</v>
+        <v>45957</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1993,10 +1995,10 @@
         <v>10</v>
       </c>
       <c r="E31" t="n">
-        <v>651.4</v>
+        <v>607.4</v>
       </c>
       <c r="F31" t="n">
-        <v>6567.59</v>
+        <v>6124.02</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -2004,15 +2006,15 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>6.49</v>
+        <v>6.08</v>
       </c>
       <c r="I31" t="n">
-        <v>47.1</v>
+        <v>43.94</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="62">
       <c r="A32" s="60" t="n">
-        <v>45950</v>
+        <v>45954</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2025,13 +2027,13 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>640.95</v>
+        <v>647.9</v>
       </c>
       <c r="F32" t="n">
-        <v>6462.21</v>
+        <v>3266.17</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2039,15 +2041,15 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>6.4</v>
+        <v>3.24</v>
       </c>
       <c r="I32" t="n">
-        <v>46.31</v>
+        <v>23.43</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="62">
       <c r="A33" s="60" t="n">
-        <v>45947</v>
+        <v>45953</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2063,10 +2065,10 @@
         <v>10</v>
       </c>
       <c r="E33" t="n">
-        <v>610.5</v>
+        <v>651.4</v>
       </c>
       <c r="F33" t="n">
-        <v>6155.25</v>
+        <v>6567.59</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2074,211 +2076,85 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>6.12</v>
+        <v>6.49</v>
       </c>
       <c r="I33" t="n">
-        <v>44.13</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="62">
-      <c r="A34" s="36" t="n">
-        <v>45807</v>
-      </c>
-      <c r="B34" s="25" t="inlineStr">
+      <c r="A34" s="60" t="n">
+        <v>45950</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>BSE</t>
         </is>
       </c>
-      <c r="C34" s="25" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
-      <c r="D34" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="E34" s="27" t="n">
-        <v>714.28</v>
-      </c>
-      <c r="F34" s="27">
-        <f>D7*E7</f>
-        <v/>
-      </c>
-      <c r="G34" s="25" t="inlineStr">
+      <c r="D34" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>640.95</v>
+      </c>
+      <c r="F34" t="n">
+        <v>6462.21</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H34" s="26" t="n"/>
-      <c r="I34" s="26" t="n"/>
-      <c r="J34" s="28">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K34" s="29">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="L34" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="M34" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
-        <v/>
-      </c>
-      <c r="N34" s="31">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
-        <v/>
-      </c>
-      <c r="O34" s="29">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="P34" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="Q34" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
-        <v/>
-      </c>
-      <c r="R34" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
-        <v/>
-      </c>
-      <c r="S34" s="32">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="T34" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="U34" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
-        <v/>
-      </c>
-      <c r="V34" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
-        <v/>
-      </c>
-      <c r="W34" s="33" t="n"/>
-      <c r="X34" s="33" t="n"/>
-      <c r="Y34" s="32">
-        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="Z34" s="33" t="n"/>
-      <c r="AA34" s="33" t="n"/>
-      <c r="AB34" s="34" t="n"/>
-      <c r="AC34" s="30">
-        <f>IF(B7="DIV", F7,"")</f>
-        <v/>
-      </c>
-      <c r="AD34" s="35" t="n"/>
+      <c r="H34" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="I34" t="n">
+        <v>46.31</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="62">
-      <c r="A35" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="B35" s="25" t="inlineStr">
+      <c r="A35" s="60" t="n">
+        <v>45947</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>BSE</t>
         </is>
       </c>
-      <c r="C35" s="25" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
-      <c r="D35" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="E35" s="27" t="n">
-        <v>699.39</v>
-      </c>
-      <c r="F35" s="27">
-        <f>D8*E8</f>
-        <v/>
-      </c>
-      <c r="G35" s="25" t="inlineStr">
+      <c r="D35" t="n">
+        <v>10</v>
+      </c>
+      <c r="E35" t="n">
+        <v>610.5</v>
+      </c>
+      <c r="F35" t="n">
+        <v>6155.25</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H35" s="26" t="n"/>
-      <c r="I35" s="26" t="n"/>
-      <c r="J35" s="28">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K35" s="29">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="L35" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
-        <v/>
-      </c>
-      <c r="M35" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
-        <v/>
-      </c>
-      <c r="N35" s="31">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
-        <v/>
-      </c>
-      <c r="O35" s="29">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="P35" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
-        <v/>
-      </c>
-      <c r="Q35" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
-        <v/>
-      </c>
-      <c r="R35" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
-        <v/>
-      </c>
-      <c r="S35" s="32">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="T35" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
-        <v/>
-      </c>
-      <c r="U35" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
-        <v/>
-      </c>
-      <c r="V35" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
-        <v/>
-      </c>
-      <c r="W35" s="33" t="n"/>
-      <c r="X35" s="33" t="n"/>
-      <c r="Y35" s="32">
-        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="Z35" s="33" t="n"/>
-      <c r="AA35" s="33" t="n"/>
-      <c r="AB35" s="34" t="n"/>
-      <c r="AC35" s="30">
-        <f>IF(B8="DIV", F8,"")</f>
-        <v/>
-      </c>
-      <c r="AD35" s="35" t="n"/>
+      <c r="H35" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="I35" t="n">
+        <v>44.13</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="62">
       <c r="A36" s="36" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="B36" s="25" t="inlineStr">
         <is>
@@ -2291,13 +2167,13 @@
         </is>
       </c>
       <c r="D36" s="26" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E36" s="27" t="n">
-        <v>702.78</v>
+        <v>714.28</v>
       </c>
       <c r="F36" s="27">
-        <f>D9*E9</f>
+        <f>D7*E7</f>
         <v/>
       </c>
       <c r="G36" s="25" t="inlineStr">
@@ -2312,64 +2188,64 @@
         <v/>
       </c>
       <c r="K36" s="29">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="L36" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="M36" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
         <v/>
       </c>
       <c r="N36" s="31">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
         <v/>
       </c>
       <c r="O36" s="29">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="P36" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="Q36" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
         <v/>
       </c>
       <c r="R36" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="S36" s="32">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="T36" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="U36" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
         <v/>
       </c>
       <c r="V36" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="W36" s="33" t="n"/>
       <c r="X36" s="33" t="n"/>
       <c r="Y36" s="32">
-        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="Z36" s="33" t="n"/>
       <c r="AA36" s="33" t="n"/>
       <c r="AB36" s="34" t="n"/>
       <c r="AC36" s="30">
-        <f>IF(B9="DIV", F9,"")</f>
+        <f>IF(B7="DIV", F7,"")</f>
         <v/>
       </c>
       <c r="AD36" s="35" t="n"/>
@@ -2389,13 +2265,13 @@
         </is>
       </c>
       <c r="D37" s="26" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E37" s="27" t="n">
-        <v>699.29</v>
+        <v>699.39</v>
       </c>
       <c r="F37" s="27">
-        <f>D10*E10</f>
+        <f>D8*E8</f>
         <v/>
       </c>
       <c r="G37" s="25" t="inlineStr">
@@ -2410,71 +2286,71 @@
         <v/>
       </c>
       <c r="K37" s="29">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="L37" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="M37" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
         <v/>
       </c>
       <c r="N37" s="31">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
         <v/>
       </c>
       <c r="O37" s="29">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="P37" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="Q37" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
         <v/>
       </c>
       <c r="R37" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="S37" s="32">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="T37" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="U37" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
         <v/>
       </c>
       <c r="V37" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="W37" s="33" t="n"/>
       <c r="X37" s="33" t="n"/>
       <c r="Y37" s="32">
-        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="Z37" s="33" t="n"/>
       <c r="AA37" s="33" t="n"/>
       <c r="AB37" s="34" t="n"/>
       <c r="AC37" s="30">
-        <f>IF(B10="DIV", F10,"")</f>
+        <f>IF(B8="DIV", F8,"")</f>
         <v/>
       </c>
       <c r="AD37" s="35" t="n"/>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="62">
       <c r="A38" s="36" t="n">
-        <v>45712</v>
+        <v>45806</v>
       </c>
       <c r="B38" s="25" t="inlineStr">
         <is>
@@ -2483,121 +2359,96 @@
       </c>
       <c r="C38" s="25" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="D38" s="26" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E38" s="27" t="n">
-        <v>484.4</v>
-      </c>
-      <c r="F38" s="27" t="n">
-        <v>968.8099999999999</v>
+        <v>702.78</v>
+      </c>
+      <c r="F38" s="27">
+        <f>D9*E9</f>
+        <v/>
       </c>
       <c r="G38" s="25" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H38" s="26" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="I38" s="26" t="n">
-        <v>6.94</v>
-      </c>
+      <c r="H38" s="26" t="n"/>
+      <c r="I38" s="26" t="n"/>
       <c r="J38" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K38" s="29">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="L38" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="M38" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
         <v/>
       </c>
       <c r="N38" s="31">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
         <v/>
       </c>
       <c r="O38" s="29">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="P38" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="Q38" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
         <v/>
       </c>
       <c r="R38" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
         <v/>
       </c>
       <c r="S38" s="32">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="T38" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="U38" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
         <v/>
       </c>
       <c r="V38" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
-        <v/>
-      </c>
-      <c r="W38" s="33" t="n">
-        <v>703.9400000000001</v>
-      </c>
-      <c r="X38" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="Y38" s="37">
-        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/SUM(F11:I11), "")</f>
-        <v/>
-      </c>
-      <c r="Z38" s="38" t="n">
-        <v>-5376.165</v>
-      </c>
-      <c r="AA38" s="38" t="n">
-        <v>5452.5</v>
-      </c>
-      <c r="AB38" s="39" t="n">
-        <v>10</v>
-      </c>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <v/>
+      </c>
+      <c r="W38" s="33" t="n"/>
+      <c r="X38" s="33" t="n"/>
+      <c r="Y38" s="32">
+        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/SUM(F9:I9), "")</f>
+        <v/>
+      </c>
+      <c r="Z38" s="33" t="n"/>
+      <c r="AA38" s="33" t="n"/>
+      <c r="AB38" s="34" t="n"/>
       <c r="AC38" s="30">
-        <f>IF(B11="DIV", F11,"")</f>
+        <f>IF(B9="DIV", F9,"")</f>
         <v/>
       </c>
       <c r="AD38" s="35" t="n"/>
-      <c r="AE38" s="40" t="n"/>
-      <c r="AF38" s="40" t="n"/>
-      <c r="AG38" s="40" t="n"/>
-      <c r="AH38" s="40" t="n"/>
-      <c r="AI38" s="40" t="n"/>
-      <c r="AJ38" s="40" t="n"/>
-      <c r="AK38" s="40" t="n"/>
-      <c r="AL38" s="40" t="n"/>
-      <c r="AM38" s="40" t="n"/>
-      <c r="AN38" s="40" t="n"/>
-      <c r="AO38" s="40" t="n"/>
-      <c r="AP38" s="40" t="n"/>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="62">
       <c r="A39" s="36" t="n">
-        <v>45712</v>
+        <v>45806</v>
       </c>
       <c r="B39" s="25" t="inlineStr">
         <is>
@@ -2606,117 +2457,92 @@
       </c>
       <c r="C39" s="25" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="D39" s="26" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E39" s="27" t="n">
-        <v>486.42</v>
-      </c>
-      <c r="F39" s="27" t="n">
-        <v>972.83</v>
+        <v>699.29</v>
+      </c>
+      <c r="F39" s="27">
+        <f>D10*E10</f>
+        <v/>
       </c>
       <c r="G39" s="25" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H39" s="26" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="I39" s="26" t="n">
-        <v>6.96</v>
-      </c>
+      <c r="H39" s="26" t="n"/>
+      <c r="I39" s="26" t="n"/>
       <c r="J39" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K39" s="29">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="L39" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="M39" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
         <v/>
       </c>
       <c r="N39" s="31">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
         <v/>
       </c>
       <c r="O39" s="29">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="P39" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="Q39" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
         <v/>
       </c>
       <c r="R39" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
         <v/>
       </c>
       <c r="S39" s="32">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="T39" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="U39" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
         <v/>
       </c>
       <c r="V39" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
-        <v/>
-      </c>
-      <c r="W39" s="33" t="n">
-        <v>703.9400000000001</v>
-      </c>
-      <c r="X39" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="Y39" s="37">
-        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/SUM(F12:I12), "")</f>
-        <v/>
-      </c>
-      <c r="Z39" s="38" t="n">
-        <v>-5412.154</v>
-      </c>
-      <c r="AA39" s="38" t="n">
-        <v>5489</v>
-      </c>
-      <c r="AB39" s="39" t="n">
-        <v>10</v>
-      </c>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <v/>
+      </c>
+      <c r="W39" s="33" t="n"/>
+      <c r="X39" s="33" t="n"/>
+      <c r="Y39" s="32">
+        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/SUM(F10:I10), "")</f>
+        <v/>
+      </c>
+      <c r="Z39" s="33" t="n"/>
+      <c r="AA39" s="33" t="n"/>
+      <c r="AB39" s="34" t="n"/>
       <c r="AC39" s="30">
-        <f>IF(B12="DIV", F12,"")</f>
+        <f>IF(B10="DIV", F10,"")</f>
         <v/>
       </c>
       <c r="AD39" s="35" t="n"/>
-      <c r="AE39" s="40" t="n"/>
-      <c r="AF39" s="40" t="n"/>
-      <c r="AG39" s="40" t="n"/>
-      <c r="AH39" s="40" t="n"/>
-      <c r="AI39" s="40" t="n"/>
-      <c r="AJ39" s="40" t="n"/>
-      <c r="AK39" s="40" t="n"/>
-      <c r="AL39" s="40" t="n"/>
-      <c r="AM39" s="40" t="n"/>
-      <c r="AN39" s="40" t="n"/>
-      <c r="AO39" s="40" t="n"/>
-      <c r="AP39" s="40" t="n"/>
     </row>
     <row r="40" ht="15.75" customHeight="1" s="62">
       <c r="A40" s="36" t="n">
@@ -2736,10 +2562,10 @@
         <v>2</v>
       </c>
       <c r="E40" s="27" t="n">
-        <v>485.17</v>
+        <v>484.4</v>
       </c>
       <c r="F40" s="27" t="n">
-        <v>970.33</v>
+        <v>968.8099999999999</v>
       </c>
       <c r="G40" s="25" t="inlineStr">
         <is>
@@ -2750,58 +2576,58 @@
         <v>0.97</v>
       </c>
       <c r="I40" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J40" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K40" s="29">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="L40" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="M40" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
         <v/>
       </c>
       <c r="N40" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
         <v/>
       </c>
       <c r="O40" s="29">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="P40" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="Q40" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
         <v/>
       </c>
       <c r="R40" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="S40" s="32">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="T40" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="U40" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
         <v/>
       </c>
       <c r="V40" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="W40" s="33" t="n">
@@ -2811,20 +2637,20 @@
         <v>45806</v>
       </c>
       <c r="Y40" s="37">
-        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="Z40" s="38" t="n">
-        <v>-5337.218</v>
+        <v>-5376.165</v>
       </c>
       <c r="AA40" s="38" t="n">
-        <v>5413</v>
+        <v>5452.5</v>
       </c>
       <c r="AB40" s="39" t="n">
         <v>10</v>
       </c>
       <c r="AC40" s="30">
-        <f>IF(B13="DIV", F13,"")</f>
+        <f>IF(B11="DIV", F11,"")</f>
         <v/>
       </c>
       <c r="AD40" s="35" t="n"/>
@@ -2859,10 +2685,10 @@
         <v>2</v>
       </c>
       <c r="E41" s="27" t="n">
-        <v>485.42</v>
+        <v>486.42</v>
       </c>
       <c r="F41" s="27" t="n">
-        <v>970.83</v>
+        <v>972.83</v>
       </c>
       <c r="G41" s="25" t="inlineStr">
         <is>
@@ -2880,51 +2706,51 @@
         <v/>
       </c>
       <c r="K41" s="29">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="L41" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="M41" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
         <v/>
       </c>
       <c r="N41" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
         <v/>
       </c>
       <c r="O41" s="29">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="P41" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="Q41" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
         <v/>
       </c>
       <c r="R41" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="S41" s="32">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="T41" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="U41" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
         <v/>
       </c>
       <c r="V41" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="W41" s="33" t="n">
@@ -2934,20 +2760,20 @@
         <v>45806</v>
       </c>
       <c r="Y41" s="37">
-        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="Z41" s="38" t="n">
-        <v>-2701.147</v>
+        <v>-5412.154</v>
       </c>
       <c r="AA41" s="38" t="n">
-        <v>2739.5</v>
+        <v>5489</v>
       </c>
       <c r="AB41" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC41" s="30">
-        <f>IF(B14="DIV", F14,"")</f>
+        <f>IF(B12="DIV", F12,"")</f>
         <v/>
       </c>
       <c r="AD41" s="35" t="n"/>
@@ -2982,10 +2808,10 @@
         <v>2</v>
       </c>
       <c r="E42" s="27" t="n">
-        <v>484.15</v>
+        <v>485.17</v>
       </c>
       <c r="F42" s="27" t="n">
-        <v>968.3099999999999</v>
+        <v>970.33</v>
       </c>
       <c r="G42" s="25" t="inlineStr">
         <is>
@@ -2996,58 +2822,58 @@
         <v>0.97</v>
       </c>
       <c r="I42" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J42" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K42" s="29">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="L42" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="M42" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
         <v/>
       </c>
       <c r="N42" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
         <v/>
       </c>
       <c r="O42" s="29">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="P42" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="Q42" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
         <v/>
       </c>
       <c r="R42" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="S42" s="32">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="T42" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="U42" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
         <v/>
       </c>
       <c r="V42" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="W42" s="33" t="n">
@@ -3057,20 +2883,20 @@
         <v>45806</v>
       </c>
       <c r="Y42" s="37">
-        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="Z42" s="38" t="n">
-        <v>-2765.4835</v>
+        <v>-5337.218</v>
       </c>
       <c r="AA42" s="38" t="n">
-        <v>2804.75</v>
+        <v>5413</v>
       </c>
       <c r="AB42" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC42" s="30">
-        <f>IF(B15="DIV", F15,"")</f>
+        <f>IF(B13="DIV", F13,"")</f>
         <v/>
       </c>
       <c r="AD42" s="35" t="n"/>
@@ -3102,13 +2928,13 @@
         </is>
       </c>
       <c r="D43" s="26" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E43" s="27" t="n">
-        <v>490.95</v>
+        <v>485.42</v>
       </c>
       <c r="F43" s="27" t="n">
-        <v>13746.59</v>
+        <v>970.83</v>
       </c>
       <c r="G43" s="25" t="inlineStr">
         <is>
@@ -3116,61 +2942,61 @@
         </is>
       </c>
       <c r="H43" s="26" t="n">
-        <v>13.53</v>
+        <v>0.97</v>
       </c>
       <c r="I43" s="26" t="n">
-        <v>98.45999999999999</v>
+        <v>6.96</v>
       </c>
       <c r="J43" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K43" s="29">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="L43" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="M43" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
         <v/>
       </c>
       <c r="N43" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
         <v/>
       </c>
       <c r="O43" s="29">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="P43" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="Q43" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
         <v/>
       </c>
       <c r="R43" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="S43" s="32">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="T43" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="U43" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
         <v/>
       </c>
       <c r="V43" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="W43" s="33" t="n">
@@ -3180,20 +3006,20 @@
         <v>45806</v>
       </c>
       <c r="Y43" s="37">
-        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="Z43" s="38" t="n">
-        <v>-2765.73</v>
+        <v>-2701.147</v>
       </c>
       <c r="AA43" s="38" t="n">
-        <v>2805</v>
+        <v>2739.5</v>
       </c>
       <c r="AB43" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC43" s="30">
-        <f>IF(B16="DIV", F16,"")</f>
+        <f>IF(B14="DIV", F14,"")</f>
         <v/>
       </c>
       <c r="AD43" s="35" t="n"/>
@@ -3228,10 +3054,10 @@
         <v>2</v>
       </c>
       <c r="E44" s="27" t="n">
-        <v>484.9</v>
+        <v>484.15</v>
       </c>
       <c r="F44" s="27" t="n">
-        <v>969.8099999999999</v>
+        <v>968.3099999999999</v>
       </c>
       <c r="G44" s="25" t="inlineStr">
         <is>
@@ -3249,51 +3075,51 @@
         <v/>
       </c>
       <c r="K44" s="29">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="L44" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="M44" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
         <v/>
       </c>
       <c r="N44" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
         <v/>
       </c>
       <c r="O44" s="29">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="P44" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="Q44" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
         <v/>
       </c>
       <c r="R44" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="S44" s="32">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="T44" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="U44" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
         <v/>
       </c>
       <c r="V44" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="W44" s="33" t="n">
@@ -3303,20 +3129,20 @@
         <v>45806</v>
       </c>
       <c r="Y44" s="37">
-        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="Z44" s="38" t="n">
-        <v>-5659.147</v>
+        <v>-2765.4835</v>
       </c>
       <c r="AA44" s="38" t="n">
-        <v>5739.5</v>
+        <v>2804.75</v>
       </c>
       <c r="AB44" s="39" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC44" s="30">
-        <f>IF(B17="DIV", F17,"")</f>
+        <f>IF(B15="DIV", F15,"")</f>
         <v/>
       </c>
       <c r="AD44" s="35" t="n"/>
@@ -3348,13 +3174,13 @@
         </is>
       </c>
       <c r="D45" s="26" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E45" s="27" t="n">
-        <v>485.67</v>
+        <v>490.95</v>
       </c>
       <c r="F45" s="27" t="n">
-        <v>971.33</v>
+        <v>13746.59</v>
       </c>
       <c r="G45" s="25" t="inlineStr">
         <is>
@@ -3362,61 +3188,61 @@
         </is>
       </c>
       <c r="H45" s="26" t="n">
-        <v>0.97</v>
+        <v>13.53</v>
       </c>
       <c r="I45" s="26" t="n">
-        <v>6.96</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="J45" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K45" s="29">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="L45" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="M45" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
         <v/>
       </c>
       <c r="N45" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
         <v/>
       </c>
       <c r="O45" s="29">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="P45" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="Q45" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
         <v/>
       </c>
       <c r="R45" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="S45" s="32">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="T45" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="U45" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
         <v/>
       </c>
       <c r="V45" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="W45" s="33" t="n">
@@ -3426,20 +3252,20 @@
         <v>45806</v>
       </c>
       <c r="Y45" s="37">
-        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="Z45" s="38" t="n">
-        <v>-2893.6635</v>
+        <v>-2765.73</v>
       </c>
       <c r="AA45" s="38" t="n">
-        <v>2934.75</v>
+        <v>2805</v>
       </c>
       <c r="AB45" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC45" s="30">
-        <f>IF(B18="DIV", F18,"")</f>
+        <f>IF(B16="DIV", F16,"")</f>
         <v/>
       </c>
       <c r="AD45" s="35" t="n"/>
@@ -3474,10 +3300,10 @@
         <v>2</v>
       </c>
       <c r="E46" s="27" t="n">
-        <v>485.92</v>
+        <v>484.9</v>
       </c>
       <c r="F46" s="27" t="n">
-        <v>971.83</v>
+        <v>969.8099999999999</v>
       </c>
       <c r="G46" s="25" t="inlineStr">
         <is>
@@ -3488,58 +3314,58 @@
         <v>0.97</v>
       </c>
       <c r="I46" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J46" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K46" s="29">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="L46" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="M46" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
         <v/>
       </c>
       <c r="N46" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
         <v/>
       </c>
       <c r="O46" s="29">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="P46" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="Q46" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
         <v/>
       </c>
       <c r="R46" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="S46" s="32">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="T46" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="U46" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
         <v/>
       </c>
       <c r="V46" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="W46" s="33" t="n">
@@ -3549,20 +3375,20 @@
         <v>45806</v>
       </c>
       <c r="Y46" s="37">
-        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="Z46" s="38" t="n">
-        <v>-3061.53</v>
+        <v>-5659.147</v>
       </c>
       <c r="AA46" s="38" t="n">
-        <v>3105</v>
+        <v>5739.5</v>
       </c>
       <c r="AB46" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC46" s="30">
-        <f>IF(B19="DIV", F19,"")</f>
+        <f>IF(B17="DIV", F17,"")</f>
         <v/>
       </c>
       <c r="AD46" s="35" t="n"/>
@@ -3597,10 +3423,10 @@
         <v>2</v>
       </c>
       <c r="E47" s="27" t="n">
-        <v>483.95</v>
+        <v>485.67</v>
       </c>
       <c r="F47" s="27" t="n">
-        <v>967.91</v>
+        <v>971.33</v>
       </c>
       <c r="G47" s="25" t="inlineStr">
         <is>
@@ -3611,58 +3437,58 @@
         <v>0.97</v>
       </c>
       <c r="I47" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J47" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K47" s="29">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="L47" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="M47" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
         <v/>
       </c>
       <c r="N47" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
         <v/>
       </c>
       <c r="O47" s="29">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="P47" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="Q47" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
         <v/>
       </c>
       <c r="R47" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="S47" s="32">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="T47" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="U47" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
         <v/>
       </c>
       <c r="V47" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="W47" s="33" t="n">
@@ -3672,20 +3498,20 @@
         <v>45806</v>
       </c>
       <c r="Y47" s="37">
-        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="Z47" s="38" t="n">
-        <v>-1232.4014</v>
+        <v>-2893.6635</v>
       </c>
       <c r="AA47" s="38" t="n">
-        <v>1249.9</v>
+        <v>2934.75</v>
       </c>
       <c r="AB47" s="39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC47" s="30">
-        <f>IF(B20="DIV", F20,"")</f>
+        <f>IF(B18="DIV", F18,"")</f>
         <v/>
       </c>
       <c r="AD47" s="35" t="n"/>
@@ -3720,10 +3546,10 @@
         <v>2</v>
       </c>
       <c r="E48" s="27" t="n">
-        <v>484.65</v>
+        <v>485.92</v>
       </c>
       <c r="F48" s="27" t="n">
-        <v>969.3099999999999</v>
+        <v>971.83</v>
       </c>
       <c r="G48" s="25" t="inlineStr">
         <is>
@@ -3734,58 +3560,58 @@
         <v>0.97</v>
       </c>
       <c r="I48" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J48" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K48" s="29">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="L48" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="M48" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
         <v/>
       </c>
       <c r="N48" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
         <v/>
       </c>
       <c r="O48" s="29">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="P48" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="Q48" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
         <v/>
       </c>
       <c r="R48" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="S48" s="32">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="T48" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="U48" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
         <v/>
       </c>
       <c r="V48" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="W48" s="33" t="n">
@@ -3795,20 +3621,20 @@
         <v>45806</v>
       </c>
       <c r="Y48" s="37">
-        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="Z48" s="38" t="n">
-        <v>-1842.2424</v>
+        <v>-3061.53</v>
       </c>
       <c r="AA48" s="38" t="n">
-        <v>1868.4</v>
+        <v>3105</v>
       </c>
       <c r="AB48" s="39" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC48" s="30">
-        <f>IF(B21="DIV", F21,"")</f>
+        <f>IF(B19="DIV", F19,"")</f>
         <v/>
       </c>
       <c r="AD48" s="35" t="n"/>
@@ -3843,10 +3669,10 @@
         <v>2</v>
       </c>
       <c r="E49" s="27" t="n">
-        <v>486.17</v>
+        <v>483.95</v>
       </c>
       <c r="F49" s="27" t="n">
-        <v>972.33</v>
+        <v>967.91</v>
       </c>
       <c r="G49" s="25" t="inlineStr">
         <is>
@@ -3857,58 +3683,58 @@
         <v>0.97</v>
       </c>
       <c r="I49" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J49" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K49" s="29">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="L49" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="M49" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
         <v/>
       </c>
       <c r="N49" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
         <v/>
       </c>
       <c r="O49" s="29">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="P49" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="Q49" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
         <v/>
       </c>
       <c r="R49" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="S49" s="32">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="T49" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="U49" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
         <v/>
       </c>
       <c r="V49" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="W49" s="33" t="n">
@@ -3918,20 +3744,20 @@
         <v>45806</v>
       </c>
       <c r="Y49" s="37">
-        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="Z49" s="38" t="n">
-        <v>-648.788</v>
+        <v>-1232.4014</v>
       </c>
       <c r="AA49" s="38" t="n">
-        <v>658</v>
+        <v>1249.9</v>
       </c>
       <c r="AB49" s="39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC49" s="30">
-        <f>IF(B22="DIV", F22,"")</f>
+        <f>IF(B20="DIV", F20,"")</f>
         <v/>
       </c>
       <c r="AD49" s="35" t="n"/>
@@ -3950,7 +3776,7 @@
     </row>
     <row r="50" ht="15.75" customHeight="1" s="62">
       <c r="A50" s="36" t="n">
-        <v>45705</v>
+        <v>45712</v>
       </c>
       <c r="B50" s="25" t="inlineStr">
         <is>
@@ -3963,13 +3789,13 @@
         </is>
       </c>
       <c r="D50" s="26" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E50" s="27" t="n">
-        <v>445.69</v>
+        <v>484.65</v>
       </c>
       <c r="F50" s="27" t="n">
-        <v>8913.73</v>
+        <v>969.3099999999999</v>
       </c>
       <c r="G50" s="25" t="inlineStr">
         <is>
@@ -3977,61 +3803,61 @@
         </is>
       </c>
       <c r="H50" s="26" t="n">
-        <v>8.83</v>
+        <v>0.97</v>
       </c>
       <c r="I50" s="26" t="n">
-        <v>63.9</v>
+        <v>6.94</v>
       </c>
       <c r="J50" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K50" s="29">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="L50" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="M50" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
         <v/>
       </c>
       <c r="N50" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
         <v/>
       </c>
       <c r="O50" s="29">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="P50" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="Q50" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
         <v/>
       </c>
       <c r="R50" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="S50" s="32">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="T50" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="U50" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
         <v/>
       </c>
       <c r="V50" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="W50" s="33" t="n">
@@ -4041,20 +3867,20 @@
         <v>45806</v>
       </c>
       <c r="Y50" s="37">
-        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="Z50" s="38" t="n">
-        <v>-1297.4774</v>
+        <v>-1842.2424</v>
       </c>
       <c r="AA50" s="38" t="n">
-        <v>1315.9</v>
+        <v>1868.4</v>
       </c>
       <c r="AB50" s="39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC50" s="30">
-        <f>IF(B23="DIV", F23,"")</f>
+        <f>IF(B21="DIV", F21,"")</f>
         <v/>
       </c>
       <c r="AD50" s="35" t="n"/>
@@ -4073,7 +3899,7 @@
     </row>
     <row r="51" ht="15.75" customHeight="1" s="62">
       <c r="A51" s="36" t="n">
-        <v>45699</v>
+        <v>45712</v>
       </c>
       <c r="B51" s="25" t="inlineStr">
         <is>
@@ -4086,13 +3912,13 @@
         </is>
       </c>
       <c r="D51" s="26" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E51" s="27" t="n">
-        <v>509.46</v>
+        <v>486.17</v>
       </c>
       <c r="F51" s="27" t="n">
-        <v>5094.65</v>
+        <v>972.33</v>
       </c>
       <c r="G51" s="25" t="inlineStr">
         <is>
@@ -4100,61 +3926,61 @@
         </is>
       </c>
       <c r="H51" s="26" t="n">
-        <v>5.05</v>
+        <v>0.97</v>
       </c>
       <c r="I51" s="26" t="n">
-        <v>36.6</v>
+        <v>6.96</v>
       </c>
       <c r="J51" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K51" s="29">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="L51" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="M51" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
         <v/>
       </c>
       <c r="N51" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
         <v/>
       </c>
       <c r="O51" s="29">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="P51" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="Q51" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
         <v/>
       </c>
       <c r="R51" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="S51" s="32">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="T51" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="U51" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
         <v/>
       </c>
       <c r="V51" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="W51" s="33" t="n">
@@ -4164,20 +3990,20 @@
         <v>45806</v>
       </c>
       <c r="Y51" s="37">
-        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="Z51" s="38" t="n">
-        <v>-1295.604</v>
+        <v>-648.788</v>
       </c>
       <c r="AA51" s="38" t="n">
-        <v>1314</v>
+        <v>658</v>
       </c>
       <c r="AB51" s="39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC51" s="30">
-        <f>IF(B24="DIV", F24,"")</f>
+        <f>IF(B22="DIV", F22,"")</f>
         <v/>
       </c>
       <c r="AD51" s="35" t="n"/>
@@ -4196,7 +4022,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1" s="62">
       <c r="A52" s="36" t="n">
-        <v>45694</v>
+        <v>45705</v>
       </c>
       <c r="B52" s="25" t="inlineStr">
         <is>
@@ -4212,10 +4038,10 @@
         <v>20</v>
       </c>
       <c r="E52" s="27" t="n">
-        <v>529.3200000000001</v>
+        <v>445.69</v>
       </c>
       <c r="F52" s="27" t="n">
-        <v>10586.46</v>
+        <v>8913.73</v>
       </c>
       <c r="G52" s="25" t="inlineStr">
         <is>
@@ -4223,61 +4049,61 @@
         </is>
       </c>
       <c r="H52" s="26" t="n">
-        <v>10.47</v>
+        <v>8.83</v>
       </c>
       <c r="I52" s="26" t="n">
-        <v>75.98999999999999</v>
+        <v>63.9</v>
       </c>
       <c r="J52" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K52" s="29">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="L52" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="M52" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
         <v/>
       </c>
       <c r="N52" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
         <v/>
       </c>
       <c r="O52" s="29">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="P52" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="Q52" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
         <v/>
       </c>
       <c r="R52" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="S52" s="32">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="T52" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="U52" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
         <v/>
       </c>
       <c r="V52" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="W52" s="33" t="n">
@@ -4287,20 +4113,20 @@
         <v>45806</v>
       </c>
       <c r="Y52" s="37">
-        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="Z52" s="38" t="n">
-        <v>-5624.637</v>
+        <v>-1297.4774</v>
       </c>
       <c r="AA52" s="38" t="n">
-        <v>5704.5</v>
+        <v>1315.9</v>
       </c>
       <c r="AB52" s="39" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AC52" s="30">
-        <f>IF(B25="DIV", F25,"")</f>
+        <f>IF(B23="DIV", F23,"")</f>
         <v/>
       </c>
       <c r="AD52" s="35" t="n"/>
@@ -4318,36 +4144,250 @@
       <c r="AP52" s="40" t="n"/>
     </row>
     <row r="53" ht="15.75" customHeight="1" s="62">
-      <c r="E53" s="41" t="n"/>
-      <c r="F53" s="41" t="n"/>
-      <c r="G53" s="42" t="n"/>
-      <c r="J53" s="41" t="n"/>
-      <c r="K53" s="41" t="n"/>
-      <c r="L53" s="41" t="n"/>
-      <c r="M53" s="1" t="n"/>
-      <c r="W53" s="41" t="n"/>
-      <c r="X53" s="41" t="n"/>
-      <c r="Y53" s="41" t="n"/>
-      <c r="Z53" s="41" t="n"/>
-      <c r="AA53" s="41" t="n"/>
-      <c r="AB53" s="41" t="n"/>
-      <c r="AC53" s="41" t="n"/>
+      <c r="A53" s="36" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B53" s="25" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C53" s="25" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D53" s="26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E53" s="27" t="n">
+        <v>509.46</v>
+      </c>
+      <c r="F53" s="27" t="n">
+        <v>5094.65</v>
+      </c>
+      <c r="G53" s="25" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H53" s="26" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I53" s="26" t="n">
+        <v>36.6</v>
+      </c>
+      <c r="J53" s="28">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K53" s="29">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="L53" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <v/>
+      </c>
+      <c r="M53" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
+        <v/>
+      </c>
+      <c r="N53" s="31">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
+        <v/>
+      </c>
+      <c r="O53" s="29">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="P53" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <v/>
+      </c>
+      <c r="Q53" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
+        <v/>
+      </c>
+      <c r="R53" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
+        <v/>
+      </c>
+      <c r="S53" s="32">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="T53" s="33">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <v/>
+      </c>
+      <c r="U53" s="33">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
+        <v/>
+      </c>
+      <c r="V53" s="33">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
+        <v/>
+      </c>
+      <c r="W53" s="33" t="n">
+        <v>703.9400000000001</v>
+      </c>
+      <c r="X53" s="36" t="n">
+        <v>45806</v>
+      </c>
+      <c r="Y53" s="37">
+        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="Z53" s="38" t="n">
+        <v>-1295.604</v>
+      </c>
+      <c r="AA53" s="38" t="n">
+        <v>1314</v>
+      </c>
+      <c r="AB53" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC53" s="30">
+        <f>IF(B24="DIV", F24,"")</f>
+        <v/>
+      </c>
+      <c r="AD53" s="35" t="n"/>
+      <c r="AE53" s="40" t="n"/>
+      <c r="AF53" s="40" t="n"/>
+      <c r="AG53" s="40" t="n"/>
+      <c r="AH53" s="40" t="n"/>
+      <c r="AI53" s="40" t="n"/>
+      <c r="AJ53" s="40" t="n"/>
+      <c r="AK53" s="40" t="n"/>
+      <c r="AL53" s="40" t="n"/>
+      <c r="AM53" s="40" t="n"/>
+      <c r="AN53" s="40" t="n"/>
+      <c r="AO53" s="40" t="n"/>
+      <c r="AP53" s="40" t="n"/>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="62">
-      <c r="E54" s="41" t="n"/>
-      <c r="F54" s="41" t="n"/>
-      <c r="G54" s="42" t="n"/>
-      <c r="J54" s="41" t="n"/>
-      <c r="K54" s="41" t="n"/>
-      <c r="L54" s="41" t="n"/>
-      <c r="M54" s="1" t="n"/>
-      <c r="W54" s="41" t="n"/>
-      <c r="X54" s="41" t="n"/>
-      <c r="Y54" s="41" t="n"/>
-      <c r="Z54" s="41" t="n"/>
-      <c r="AA54" s="41" t="n"/>
-      <c r="AB54" s="41" t="n"/>
-      <c r="AC54" s="41" t="n"/>
+      <c r="A54" s="36" t="n">
+        <v>45694</v>
+      </c>
+      <c r="B54" s="25" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C54" s="25" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D54" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="E54" s="27" t="n">
+        <v>529.3200000000001</v>
+      </c>
+      <c r="F54" s="27" t="n">
+        <v>10586.46</v>
+      </c>
+      <c r="G54" s="25" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H54" s="26" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="I54" s="26" t="n">
+        <v>75.98999999999999</v>
+      </c>
+      <c r="J54" s="28">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K54" s="29">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="L54" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="M54" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <v/>
+      </c>
+      <c r="N54" s="31">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <v/>
+      </c>
+      <c r="O54" s="29">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="P54" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="Q54" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <v/>
+      </c>
+      <c r="R54" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <v/>
+      </c>
+      <c r="S54" s="32">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="T54" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="U54" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <v/>
+      </c>
+      <c r="V54" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <v/>
+      </c>
+      <c r="W54" s="33" t="n">
+        <v>703.9400000000001</v>
+      </c>
+      <c r="X54" s="36" t="n">
+        <v>45806</v>
+      </c>
+      <c r="Y54" s="37">
+        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="Z54" s="38" t="n">
+        <v>-5624.637</v>
+      </c>
+      <c r="AA54" s="38" t="n">
+        <v>5704.5</v>
+      </c>
+      <c r="AB54" s="39" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC54" s="30">
+        <f>IF(B25="DIV", F25,"")</f>
+        <v/>
+      </c>
+      <c r="AD54" s="35" t="n"/>
+      <c r="AE54" s="40" t="n"/>
+      <c r="AF54" s="40" t="n"/>
+      <c r="AG54" s="40" t="n"/>
+      <c r="AH54" s="40" t="n"/>
+      <c r="AI54" s="40" t="n"/>
+      <c r="AJ54" s="40" t="n"/>
+      <c r="AK54" s="40" t="n"/>
+      <c r="AL54" s="40" t="n"/>
+      <c r="AM54" s="40" t="n"/>
+      <c r="AN54" s="40" t="n"/>
+      <c r="AO54" s="40" t="n"/>
+      <c r="AP54" s="40" t="n"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="62">
       <c r="E55" s="41" t="n"/>
@@ -19300,6 +19340,7 @@
       <c r="J989" s="41" t="n"/>
       <c r="K989" s="41" t="n"/>
       <c r="L989" s="41" t="n"/>
+      <c r="M989" s="1" t="n"/>
       <c r="W989" s="41" t="n"/>
       <c r="X989" s="41" t="n"/>
       <c r="Y989" s="41" t="n"/>
@@ -19315,6 +19356,7 @@
       <c r="J990" s="41" t="n"/>
       <c r="K990" s="41" t="n"/>
       <c r="L990" s="41" t="n"/>
+      <c r="M990" s="1" t="n"/>
       <c r="W990" s="41" t="n"/>
       <c r="X990" s="41" t="n"/>
       <c r="Y990" s="41" t="n"/>
@@ -19547,6 +19589,36 @@
       <c r="AA1005" s="41" t="n"/>
       <c r="AB1005" s="41" t="n"/>
       <c r="AC1005" s="41" t="n"/>
+    </row>
+    <row r="1006">
+      <c r="E1006" s="41" t="n"/>
+      <c r="F1006" s="41" t="n"/>
+      <c r="G1006" s="42" t="n"/>
+      <c r="J1006" s="41" t="n"/>
+      <c r="K1006" s="41" t="n"/>
+      <c r="L1006" s="41" t="n"/>
+      <c r="W1006" s="41" t="n"/>
+      <c r="X1006" s="41" t="n"/>
+      <c r="Y1006" s="41" t="n"/>
+      <c r="Z1006" s="41" t="n"/>
+      <c r="AA1006" s="41" t="n"/>
+      <c r="AB1006" s="41" t="n"/>
+      <c r="AC1006" s="41" t="n"/>
+    </row>
+    <row r="1007">
+      <c r="E1007" s="41" t="n"/>
+      <c r="F1007" s="41" t="n"/>
+      <c r="G1007" s="42" t="n"/>
+      <c r="J1007" s="41" t="n"/>
+      <c r="K1007" s="41" t="n"/>
+      <c r="L1007" s="41" t="n"/>
+      <c r="W1007" s="41" t="n"/>
+      <c r="X1007" s="41" t="n"/>
+      <c r="Y1007" s="41" t="n"/>
+      <c r="Z1007" s="41" t="n"/>
+      <c r="AA1007" s="41" t="n"/>
+      <c r="AB1007" s="41" t="n"/>
+      <c r="AC1007" s="41" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:AO53"/>

</xml_diff>

<commit_message>
Update additional stock data files
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/High Energy Batteries (India) Ltd.xlsx
+++ b/dumps/Stocks/High Energy Batteries (India) Ltd.xlsx
@@ -712,7 +712,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1007"/>
+  <dimension ref="A1:AP1008"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" s="62">
       <c r="A5" s="73" t="n">
-        <v>45967</v>
+        <v>45978</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1075,21 +1075,21 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>570.45</v>
+        <v>657.58</v>
       </c>
       <c r="F5" t="n">
-        <v>5733</v>
+        <v>3304.35</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CN#252607785263</t>
+          <t>CN#252608260909</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>28.5</v>
+        <v>16.45</v>
       </c>
       <c r="J5">
         <f>Index!$C$2</f>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" s="62">
       <c r="A6" s="73" t="n">
-        <v>45961</v>
+        <v>45967</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1111,21 +1111,21 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>596.15</v>
+        <v>570.45</v>
       </c>
       <c r="F6" t="n">
-        <v>2995.65</v>
+        <v>5733</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>CN#252607606298</t>
+          <t>CN#252607785263</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>14.9</v>
+        <v>28.5</v>
       </c>
       <c r="J6">
         <f>Index!$C$2</f>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" s="62">
       <c r="A7" s="73" t="n">
-        <v>45957</v>
+        <v>45961</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1147,21 +1147,21 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>607.4</v>
+        <v>596.15</v>
       </c>
       <c r="F7" t="n">
-        <v>6104.4</v>
+        <v>2995.65</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>CN#252607382790</t>
+          <t>CN#252607606298</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>30.4</v>
+        <v>14.9</v>
       </c>
       <c r="J7">
         <f>Index!$C$2</f>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1" s="62">
       <c r="A8" s="73" t="n">
-        <v>46063</v>
+        <v>45957</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1186,21 +1186,18 @@
         <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>589.75</v>
+        <v>607.4</v>
       </c>
       <c r="F8" t="n">
-        <v>5946.05</v>
+        <v>6104.4</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CN#252611730667</t>
+          <t>CN#252607382790</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>5.89</v>
-      </c>
       <c r="I8" t="n">
-        <v>42.66</v>
+        <v>30.4</v>
       </c>
       <c r="J8">
         <f>Index!$C$2</f>
@@ -1208,8 +1205,8 @@
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="62">
-      <c r="A9" s="60" t="n">
-        <v>46050</v>
+      <c r="A9" s="73" t="n">
+        <v>46063</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1225,26 +1222,30 @@
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>530</v>
+        <v>589.75</v>
       </c>
       <c r="F9" t="n">
-        <v>5343.69</v>
+        <v>5946.05</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>CN#252611730667</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>5.33</v>
+        <v>5.89</v>
       </c>
       <c r="I9" t="n">
-        <v>38.36</v>
+        <v>42.66</v>
+      </c>
+      <c r="J9">
+        <f>Index!$C$2</f>
+        <v/>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="62">
       <c r="A10" s="60" t="n">
-        <v>46049</v>
+        <v>46050</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1257,13 +1258,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>534.7</v>
+        <v>530</v>
       </c>
       <c r="F10" t="n">
-        <v>2695.48</v>
+        <v>5343.69</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1271,15 +1272,15 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>2.67</v>
+        <v>5.33</v>
       </c>
       <c r="I10" t="n">
-        <v>19.31</v>
+        <v>38.36</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="62">
       <c r="A11" s="60" t="n">
-        <v>46042</v>
+        <v>46049</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1292,13 +1293,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
-        <v>541</v>
+        <v>534.7</v>
       </c>
       <c r="F11" t="n">
-        <v>5454.64</v>
+        <v>2695.48</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1306,15 +1307,15 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>5.42</v>
+        <v>2.67</v>
       </c>
       <c r="I11" t="n">
-        <v>39.22</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="62">
       <c r="A12" s="60" t="n">
-        <v>46030</v>
+        <v>46042</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1330,10 +1331,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>563.85</v>
+        <v>541</v>
       </c>
       <c r="F12" t="n">
-        <v>5684.91</v>
+        <v>5454.64</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1341,15 +1342,15 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>5.62</v>
+        <v>5.42</v>
       </c>
       <c r="I12" t="n">
-        <v>40.79</v>
+        <v>39.22</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="62">
       <c r="A13" s="60" t="n">
-        <v>46017</v>
+        <v>46030</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1362,13 +1363,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
-        <v>545.55</v>
+        <v>563.85</v>
       </c>
       <c r="F13" t="n">
-        <v>2750.24</v>
+        <v>5684.91</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1376,10 +1377,10 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>2.74</v>
+        <v>5.62</v>
       </c>
       <c r="I13" t="n">
-        <v>19.75</v>
+        <v>40.79</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="62">
@@ -1400,10 +1401,10 @@
         <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>545.5</v>
+        <v>545.55</v>
       </c>
       <c r="F14" t="n">
-        <v>2749.99</v>
+        <v>2750.24</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1419,7 +1420,7 @@
     </row>
     <row r="15" ht="15.75" customHeight="1" s="62">
       <c r="A15" s="60" t="n">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1432,13 +1433,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>545.25</v>
+        <v>545.5</v>
       </c>
       <c r="F15" t="n">
-        <v>5497.42</v>
+        <v>2749.99</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1446,15 +1447,15 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>5.42</v>
+        <v>2.74</v>
       </c>
       <c r="I15" t="n">
-        <v>39.5</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="62">
       <c r="A16" s="60" t="n">
-        <v>46014</v>
+        <v>46015</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1470,10 +1471,10 @@
         <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>548.9</v>
+        <v>545.25</v>
       </c>
       <c r="F16" t="n">
-        <v>5534.11</v>
+        <v>5497.42</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1481,15 +1482,15 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>5.47</v>
+        <v>5.42</v>
       </c>
       <c r="I16" t="n">
-        <v>39.64</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="62">
       <c r="A17" s="60" t="n">
-        <v>46007</v>
+        <v>46014</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1505,10 +1506,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>541.3</v>
+        <v>548.9</v>
       </c>
       <c r="F17" t="n">
-        <v>5457.59</v>
+        <v>5534.11</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1516,15 +1517,15 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>5.39</v>
+        <v>5.47</v>
       </c>
       <c r="I17" t="n">
-        <v>39.2</v>
+        <v>39.64</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="62">
       <c r="A18" s="60" t="n">
-        <v>46002</v>
+        <v>46007</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1537,13 +1538,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>547.9</v>
+        <v>541.3</v>
       </c>
       <c r="F18" t="n">
-        <v>2762.01</v>
+        <v>5457.59</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1551,15 +1552,15 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>2.75</v>
+        <v>5.39</v>
       </c>
       <c r="I18" t="n">
-        <v>19.76</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="62">
       <c r="A19" s="60" t="n">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1575,10 +1576,10 @@
         <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>560.95</v>
+        <v>547.9</v>
       </c>
       <c r="F19" t="n">
-        <v>2827.8</v>
+        <v>2762.01</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1586,10 +1587,10 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>2.8</v>
+        <v>2.75</v>
       </c>
       <c r="I19" t="n">
-        <v>20.25</v>
+        <v>19.76</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="62">
@@ -1610,10 +1611,10 @@
         <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>561</v>
+        <v>560.95</v>
       </c>
       <c r="F20" t="n">
-        <v>2828.11</v>
+        <v>2827.8</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1624,12 +1625,12 @@
         <v>2.8</v>
       </c>
       <c r="I20" t="n">
-        <v>20.31</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="62">
       <c r="A21" s="60" t="n">
-        <v>45996</v>
+        <v>46000</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1642,13 +1643,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>573.95</v>
+        <v>561</v>
       </c>
       <c r="F21" t="n">
-        <v>5786.76</v>
+        <v>2828.11</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1656,15 +1657,15 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>5.72</v>
+        <v>2.8</v>
       </c>
       <c r="I21" t="n">
-        <v>41.54</v>
+        <v>20.31</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="62">
       <c r="A22" s="60" t="n">
-        <v>45989</v>
+        <v>45996</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1677,13 +1678,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>586.95</v>
+        <v>573.95</v>
       </c>
       <c r="F22" t="n">
-        <v>2958.88</v>
+        <v>5786.76</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1691,15 +1692,15 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>2.93</v>
+        <v>5.72</v>
       </c>
       <c r="I22" t="n">
-        <v>21.2</v>
+        <v>41.54</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="62">
       <c r="A23" s="60" t="n">
-        <v>45982</v>
+        <v>45989</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1715,10 +1716,10 @@
         <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>621</v>
+        <v>586.95</v>
       </c>
       <c r="F23" t="n">
-        <v>3130.59</v>
+        <v>2958.88</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1726,15 +1727,15 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>3.11</v>
+        <v>2.93</v>
       </c>
       <c r="I23" t="n">
-        <v>22.48</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="62">
       <c r="A24" s="60" t="n">
-        <v>45979</v>
+        <v>45982</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1747,13 +1748,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E24" t="n">
-        <v>624.95</v>
+        <v>621</v>
       </c>
       <c r="F24" t="n">
-        <v>1260.17</v>
+        <v>3130.59</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1761,10 +1762,10 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>1.25</v>
+        <v>3.11</v>
       </c>
       <c r="I24" t="n">
-        <v>9.02</v>
+        <v>22.48</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="62">
@@ -1782,13 +1783,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" t="n">
-        <v>622.8</v>
+        <v>624.95</v>
       </c>
       <c r="F25" t="n">
-        <v>1883.78</v>
+        <v>1260.17</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1796,15 +1797,15 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>1.88</v>
+        <v>1.25</v>
       </c>
       <c r="I25" t="n">
-        <v>13.5</v>
+        <v>9.02</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="62">
       <c r="A26" s="60" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1817,13 +1818,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
-        <v>658</v>
+        <v>622.8</v>
       </c>
       <c r="F26" t="n">
-        <v>663.4299999999999</v>
+        <v>1883.78</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1831,10 +1832,10 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>0.66</v>
+        <v>1.88</v>
       </c>
       <c r="I26" t="n">
-        <v>4.77</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="62">
@@ -1852,13 +1853,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>657.95</v>
+        <v>658</v>
       </c>
       <c r="F27" t="n">
-        <v>1326.73</v>
+        <v>663.4299999999999</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1866,10 +1867,10 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>1.32</v>
+        <v>0.66</v>
       </c>
       <c r="I27" t="n">
-        <v>9.51</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="62">
@@ -1890,10 +1891,10 @@
         <v>2</v>
       </c>
       <c r="E28" t="n">
-        <v>657</v>
+        <v>657.95</v>
       </c>
       <c r="F28" t="n">
-        <v>1324.82</v>
+        <v>1326.73</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1904,12 +1905,12 @@
         <v>1.32</v>
       </c>
       <c r="I28" t="n">
-        <v>9.5</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="62">
       <c r="A29" s="60" t="n">
-        <v>45967</v>
+        <v>45978</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1922,13 +1923,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>570.45</v>
+        <v>657</v>
       </c>
       <c r="F29" t="n">
-        <v>5751.49</v>
+        <v>1324.82</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1936,15 +1937,15 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>5.74</v>
+        <v>1.32</v>
       </c>
       <c r="I29" t="n">
-        <v>41.25</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="62">
       <c r="A30" s="60" t="n">
-        <v>45961</v>
+        <v>45967</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1957,13 +1958,13 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>596.15</v>
+        <v>570.45</v>
       </c>
       <c r="F30" t="n">
-        <v>3005.27</v>
+        <v>5751.49</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1971,15 +1972,15 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>2.97</v>
+        <v>5.74</v>
       </c>
       <c r="I30" t="n">
-        <v>21.55</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="62">
       <c r="A31" s="60" t="n">
-        <v>45957</v>
+        <v>45961</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1992,13 +1993,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E31" t="n">
-        <v>607.4</v>
+        <v>596.15</v>
       </c>
       <c r="F31" t="n">
-        <v>6124.02</v>
+        <v>3005.27</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -2006,15 +2007,15 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>6.08</v>
+        <v>2.97</v>
       </c>
       <c r="I31" t="n">
-        <v>43.94</v>
+        <v>21.55</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="62">
       <c r="A32" s="60" t="n">
-        <v>45954</v>
+        <v>45957</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2027,13 +2028,13 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>647.9</v>
+        <v>607.4</v>
       </c>
       <c r="F32" t="n">
-        <v>3266.17</v>
+        <v>6124.02</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2041,15 +2042,15 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>3.24</v>
+        <v>6.08</v>
       </c>
       <c r="I32" t="n">
-        <v>23.43</v>
+        <v>43.94</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="62">
       <c r="A33" s="60" t="n">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2062,13 +2063,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E33" t="n">
-        <v>651.4</v>
+        <v>647.9</v>
       </c>
       <c r="F33" t="n">
-        <v>6567.59</v>
+        <v>3266.17</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2076,15 +2077,15 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>6.49</v>
+        <v>3.24</v>
       </c>
       <c r="I33" t="n">
-        <v>47.1</v>
+        <v>23.43</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="62">
       <c r="A34" s="60" t="n">
-        <v>45950</v>
+        <v>45953</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2100,10 +2101,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>640.95</v>
+        <v>651.4</v>
       </c>
       <c r="F34" t="n">
-        <v>6462.21</v>
+        <v>6567.59</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2111,15 +2112,15 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>6.4</v>
+        <v>6.49</v>
       </c>
       <c r="I34" t="n">
-        <v>46.31</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="62">
       <c r="A35" s="60" t="n">
-        <v>45947</v>
+        <v>45950</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2135,10 +2136,10 @@
         <v>10</v>
       </c>
       <c r="E35" t="n">
-        <v>610.5</v>
+        <v>640.95</v>
       </c>
       <c r="F35" t="n">
-        <v>6155.25</v>
+        <v>6462.21</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2146,113 +2147,50 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>6.12</v>
+        <v>6.4</v>
       </c>
       <c r="I35" t="n">
-        <v>44.13</v>
+        <v>46.31</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="62">
-      <c r="A36" s="36" t="n">
-        <v>45807</v>
-      </c>
-      <c r="B36" s="25" t="inlineStr">
+      <c r="A36" s="60" t="n">
+        <v>45947</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>BSE</t>
         </is>
       </c>
-      <c r="C36" s="25" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
-      <c r="D36" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="E36" s="27" t="n">
-        <v>714.28</v>
-      </c>
-      <c r="F36" s="27">
-        <f>D7*E7</f>
-        <v/>
-      </c>
-      <c r="G36" s="25" t="inlineStr">
+      <c r="D36" t="n">
+        <v>10</v>
+      </c>
+      <c r="E36" t="n">
+        <v>610.5</v>
+      </c>
+      <c r="F36" t="n">
+        <v>6155.25</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H36" s="26" t="n"/>
-      <c r="I36" s="26" t="n"/>
-      <c r="J36" s="28">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K36" s="29">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="L36" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="M36" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
-        <v/>
-      </c>
-      <c r="N36" s="31">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
-        <v/>
-      </c>
-      <c r="O36" s="29">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="P36" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="Q36" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
-        <v/>
-      </c>
-      <c r="R36" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
-        <v/>
-      </c>
-      <c r="S36" s="32">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="T36" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="U36" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
-        <v/>
-      </c>
-      <c r="V36" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
-        <v/>
-      </c>
-      <c r="W36" s="33" t="n"/>
-      <c r="X36" s="33" t="n"/>
-      <c r="Y36" s="32">
-        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="Z36" s="33" t="n"/>
-      <c r="AA36" s="33" t="n"/>
-      <c r="AB36" s="34" t="n"/>
-      <c r="AC36" s="30">
-        <f>IF(B7="DIV", F7,"")</f>
-        <v/>
-      </c>
-      <c r="AD36" s="35" t="n"/>
+      <c r="H36" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="I36" t="n">
+        <v>44.13</v>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="62">
       <c r="A37" s="36" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="B37" s="25" t="inlineStr">
         <is>
@@ -2265,13 +2203,13 @@
         </is>
       </c>
       <c r="D37" s="26" t="n">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E37" s="27" t="n">
-        <v>699.39</v>
+        <v>714.28</v>
       </c>
       <c r="F37" s="27">
-        <f>D8*E8</f>
+        <f>D7*E7</f>
         <v/>
       </c>
       <c r="G37" s="25" t="inlineStr">
@@ -2286,64 +2224,64 @@
         <v/>
       </c>
       <c r="K37" s="29">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/SUM(F8:I8), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="L37" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="M37" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
         <v/>
       </c>
       <c r="N37" s="31">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
         <v/>
       </c>
       <c r="O37" s="29">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/SUM(F8:I8), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="P37" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="Q37" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
         <v/>
       </c>
       <c r="R37" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="S37" s="32">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/SUM(F8:I8), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="T37" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="U37" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
         <v/>
       </c>
       <c r="V37" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="W37" s="33" t="n"/>
       <c r="X37" s="33" t="n"/>
       <c r="Y37" s="32">
-        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/SUM(F8:I8), "")</f>
+        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="Z37" s="33" t="n"/>
       <c r="AA37" s="33" t="n"/>
       <c r="AB37" s="34" t="n"/>
       <c r="AC37" s="30">
-        <f>IF(B8="DIV", F8,"")</f>
+        <f>IF(B7="DIV", F7,"")</f>
         <v/>
       </c>
       <c r="AD37" s="35" t="n"/>
@@ -2363,13 +2301,13 @@
         </is>
       </c>
       <c r="D38" s="26" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E38" s="27" t="n">
-        <v>702.78</v>
+        <v>699.39</v>
       </c>
       <c r="F38" s="27">
-        <f>D9*E9</f>
+        <f>D8*E8</f>
         <v/>
       </c>
       <c r="G38" s="25" t="inlineStr">
@@ -2384,64 +2322,64 @@
         <v/>
       </c>
       <c r="K38" s="29">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="L38" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="M38" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
         <v/>
       </c>
       <c r="N38" s="31">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
         <v/>
       </c>
       <c r="O38" s="29">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="P38" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="Q38" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
         <v/>
       </c>
       <c r="R38" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="S38" s="32">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="T38" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="U38" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
         <v/>
       </c>
       <c r="V38" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="W38" s="33" t="n"/>
       <c r="X38" s="33" t="n"/>
       <c r="Y38" s="32">
-        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="Z38" s="33" t="n"/>
       <c r="AA38" s="33" t="n"/>
       <c r="AB38" s="34" t="n"/>
       <c r="AC38" s="30">
-        <f>IF(B9="DIV", F9,"")</f>
+        <f>IF(B8="DIV", F8,"")</f>
         <v/>
       </c>
       <c r="AD38" s="35" t="n"/>
@@ -2461,13 +2399,13 @@
         </is>
       </c>
       <c r="D39" s="26" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E39" s="27" t="n">
-        <v>699.29</v>
+        <v>702.78</v>
       </c>
       <c r="F39" s="27">
-        <f>D10*E10</f>
+        <f>D9*E9</f>
         <v/>
       </c>
       <c r="G39" s="25" t="inlineStr">
@@ -2482,71 +2420,71 @@
         <v/>
       </c>
       <c r="K39" s="29">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="L39" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="M39" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
         <v/>
       </c>
       <c r="N39" s="31">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
         <v/>
       </c>
       <c r="O39" s="29">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="P39" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="Q39" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
         <v/>
       </c>
       <c r="R39" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
         <v/>
       </c>
       <c r="S39" s="32">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="T39" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="U39" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
         <v/>
       </c>
       <c r="V39" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
         <v/>
       </c>
       <c r="W39" s="33" t="n"/>
       <c r="X39" s="33" t="n"/>
       <c r="Y39" s="32">
-        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="Z39" s="33" t="n"/>
       <c r="AA39" s="33" t="n"/>
       <c r="AB39" s="34" t="n"/>
       <c r="AC39" s="30">
-        <f>IF(B10="DIV", F10,"")</f>
+        <f>IF(B9="DIV", F9,"")</f>
         <v/>
       </c>
       <c r="AD39" s="35" t="n"/>
     </row>
     <row r="40" ht="15.75" customHeight="1" s="62">
       <c r="A40" s="36" t="n">
-        <v>45712</v>
+        <v>45806</v>
       </c>
       <c r="B40" s="25" t="inlineStr">
         <is>
@@ -2555,117 +2493,92 @@
       </c>
       <c r="C40" s="25" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="D40" s="26" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E40" s="27" t="n">
-        <v>484.4</v>
-      </c>
-      <c r="F40" s="27" t="n">
-        <v>968.8099999999999</v>
+        <v>699.29</v>
+      </c>
+      <c r="F40" s="27">
+        <f>D10*E10</f>
+        <v/>
       </c>
       <c r="G40" s="25" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H40" s="26" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="I40" s="26" t="n">
-        <v>6.94</v>
-      </c>
+      <c r="H40" s="26" t="n"/>
+      <c r="I40" s="26" t="n"/>
       <c r="J40" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K40" s="29">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="L40" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="M40" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
         <v/>
       </c>
       <c r="N40" s="31">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
         <v/>
       </c>
       <c r="O40" s="29">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="P40" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="Q40" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
         <v/>
       </c>
       <c r="R40" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
         <v/>
       </c>
       <c r="S40" s="32">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="T40" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="U40" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
         <v/>
       </c>
       <c r="V40" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
-        <v/>
-      </c>
-      <c r="W40" s="33" t="n">
-        <v>703.9400000000001</v>
-      </c>
-      <c r="X40" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="Y40" s="37">
-        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/SUM(F11:I11), "")</f>
-        <v/>
-      </c>
-      <c r="Z40" s="38" t="n">
-        <v>-5376.165</v>
-      </c>
-      <c r="AA40" s="38" t="n">
-        <v>5452.5</v>
-      </c>
-      <c r="AB40" s="39" t="n">
-        <v>10</v>
-      </c>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <v/>
+      </c>
+      <c r="W40" s="33" t="n"/>
+      <c r="X40" s="33" t="n"/>
+      <c r="Y40" s="32">
+        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/SUM(F10:I10), "")</f>
+        <v/>
+      </c>
+      <c r="Z40" s="33" t="n"/>
+      <c r="AA40" s="33" t="n"/>
+      <c r="AB40" s="34" t="n"/>
       <c r="AC40" s="30">
-        <f>IF(B11="DIV", F11,"")</f>
+        <f>IF(B10="DIV", F10,"")</f>
         <v/>
       </c>
       <c r="AD40" s="35" t="n"/>
-      <c r="AE40" s="40" t="n"/>
-      <c r="AF40" s="40" t="n"/>
-      <c r="AG40" s="40" t="n"/>
-      <c r="AH40" s="40" t="n"/>
-      <c r="AI40" s="40" t="n"/>
-      <c r="AJ40" s="40" t="n"/>
-      <c r="AK40" s="40" t="n"/>
-      <c r="AL40" s="40" t="n"/>
-      <c r="AM40" s="40" t="n"/>
-      <c r="AN40" s="40" t="n"/>
-      <c r="AO40" s="40" t="n"/>
-      <c r="AP40" s="40" t="n"/>
     </row>
     <row r="41" ht="15.75" customHeight="1" s="62">
       <c r="A41" s="36" t="n">
@@ -2685,10 +2598,10 @@
         <v>2</v>
       </c>
       <c r="E41" s="27" t="n">
-        <v>486.42</v>
+        <v>484.4</v>
       </c>
       <c r="F41" s="27" t="n">
-        <v>972.83</v>
+        <v>968.8099999999999</v>
       </c>
       <c r="G41" s="25" t="inlineStr">
         <is>
@@ -2699,58 +2612,58 @@
         <v>0.97</v>
       </c>
       <c r="I41" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J41" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K41" s="29">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="L41" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="M41" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
         <v/>
       </c>
       <c r="N41" s="31">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
         <v/>
       </c>
       <c r="O41" s="29">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="P41" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="Q41" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
         <v/>
       </c>
       <c r="R41" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="S41" s="32">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="T41" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="U41" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
         <v/>
       </c>
       <c r="V41" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="W41" s="33" t="n">
@@ -2760,20 +2673,20 @@
         <v>45806</v>
       </c>
       <c r="Y41" s="37">
-        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="Z41" s="38" t="n">
-        <v>-5412.154</v>
+        <v>-5376.165</v>
       </c>
       <c r="AA41" s="38" t="n">
-        <v>5489</v>
+        <v>5452.5</v>
       </c>
       <c r="AB41" s="39" t="n">
         <v>10</v>
       </c>
       <c r="AC41" s="30">
-        <f>IF(B12="DIV", F12,"")</f>
+        <f>IF(B11="DIV", F11,"")</f>
         <v/>
       </c>
       <c r="AD41" s="35" t="n"/>
@@ -2808,10 +2721,10 @@
         <v>2</v>
       </c>
       <c r="E42" s="27" t="n">
-        <v>485.17</v>
+        <v>486.42</v>
       </c>
       <c r="F42" s="27" t="n">
-        <v>970.33</v>
+        <v>972.83</v>
       </c>
       <c r="G42" s="25" t="inlineStr">
         <is>
@@ -2829,51 +2742,51 @@
         <v/>
       </c>
       <c r="K42" s="29">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="L42" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="M42" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
         <v/>
       </c>
       <c r="N42" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
         <v/>
       </c>
       <c r="O42" s="29">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="P42" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="Q42" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
         <v/>
       </c>
       <c r="R42" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="S42" s="32">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="T42" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="U42" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
         <v/>
       </c>
       <c r="V42" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="W42" s="33" t="n">
@@ -2883,20 +2796,20 @@
         <v>45806</v>
       </c>
       <c r="Y42" s="37">
-        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="Z42" s="38" t="n">
-        <v>-5337.218</v>
+        <v>-5412.154</v>
       </c>
       <c r="AA42" s="38" t="n">
-        <v>5413</v>
+        <v>5489</v>
       </c>
       <c r="AB42" s="39" t="n">
         <v>10</v>
       </c>
       <c r="AC42" s="30">
-        <f>IF(B13="DIV", F13,"")</f>
+        <f>IF(B12="DIV", F12,"")</f>
         <v/>
       </c>
       <c r="AD42" s="35" t="n"/>
@@ -2931,10 +2844,10 @@
         <v>2</v>
       </c>
       <c r="E43" s="27" t="n">
-        <v>485.42</v>
+        <v>485.17</v>
       </c>
       <c r="F43" s="27" t="n">
-        <v>970.83</v>
+        <v>970.33</v>
       </c>
       <c r="G43" s="25" t="inlineStr">
         <is>
@@ -2952,51 +2865,51 @@
         <v/>
       </c>
       <c r="K43" s="29">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="L43" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="M43" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
         <v/>
       </c>
       <c r="N43" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
         <v/>
       </c>
       <c r="O43" s="29">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="P43" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="Q43" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
         <v/>
       </c>
       <c r="R43" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="S43" s="32">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="T43" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="U43" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
         <v/>
       </c>
       <c r="V43" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="W43" s="33" t="n">
@@ -3006,20 +2919,20 @@
         <v>45806</v>
       </c>
       <c r="Y43" s="37">
-        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="Z43" s="38" t="n">
-        <v>-2701.147</v>
+        <v>-5337.218</v>
       </c>
       <c r="AA43" s="38" t="n">
-        <v>2739.5</v>
+        <v>5413</v>
       </c>
       <c r="AB43" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC43" s="30">
-        <f>IF(B14="DIV", F14,"")</f>
+        <f>IF(B13="DIV", F13,"")</f>
         <v/>
       </c>
       <c r="AD43" s="35" t="n"/>
@@ -3054,10 +2967,10 @@
         <v>2</v>
       </c>
       <c r="E44" s="27" t="n">
-        <v>484.15</v>
+        <v>485.42</v>
       </c>
       <c r="F44" s="27" t="n">
-        <v>968.3099999999999</v>
+        <v>970.83</v>
       </c>
       <c r="G44" s="25" t="inlineStr">
         <is>
@@ -3068,58 +2981,58 @@
         <v>0.97</v>
       </c>
       <c r="I44" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J44" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K44" s="29">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="L44" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="M44" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
         <v/>
       </c>
       <c r="N44" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
         <v/>
       </c>
       <c r="O44" s="29">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="P44" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="Q44" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
         <v/>
       </c>
       <c r="R44" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="S44" s="32">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="T44" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="U44" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
         <v/>
       </c>
       <c r="V44" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="W44" s="33" t="n">
@@ -3129,20 +3042,20 @@
         <v>45806</v>
       </c>
       <c r="Y44" s="37">
-        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="Z44" s="38" t="n">
-        <v>-2765.4835</v>
+        <v>-2701.147</v>
       </c>
       <c r="AA44" s="38" t="n">
-        <v>2804.75</v>
+        <v>2739.5</v>
       </c>
       <c r="AB44" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC44" s="30">
-        <f>IF(B15="DIV", F15,"")</f>
+        <f>IF(B14="DIV", F14,"")</f>
         <v/>
       </c>
       <c r="AD44" s="35" t="n"/>
@@ -3174,13 +3087,13 @@
         </is>
       </c>
       <c r="D45" s="26" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E45" s="27" t="n">
-        <v>490.95</v>
+        <v>484.15</v>
       </c>
       <c r="F45" s="27" t="n">
-        <v>13746.59</v>
+        <v>968.3099999999999</v>
       </c>
       <c r="G45" s="25" t="inlineStr">
         <is>
@@ -3188,61 +3101,61 @@
         </is>
       </c>
       <c r="H45" s="26" t="n">
-        <v>13.53</v>
+        <v>0.97</v>
       </c>
       <c r="I45" s="26" t="n">
-        <v>98.45999999999999</v>
+        <v>6.94</v>
       </c>
       <c r="J45" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K45" s="29">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="L45" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="M45" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
         <v/>
       </c>
       <c r="N45" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
         <v/>
       </c>
       <c r="O45" s="29">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="P45" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="Q45" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
         <v/>
       </c>
       <c r="R45" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="S45" s="32">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="T45" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="U45" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
         <v/>
       </c>
       <c r="V45" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="W45" s="33" t="n">
@@ -3252,20 +3165,20 @@
         <v>45806</v>
       </c>
       <c r="Y45" s="37">
-        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="Z45" s="38" t="n">
-        <v>-2765.73</v>
+        <v>-2765.4835</v>
       </c>
       <c r="AA45" s="38" t="n">
-        <v>2805</v>
+        <v>2804.75</v>
       </c>
       <c r="AB45" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC45" s="30">
-        <f>IF(B16="DIV", F16,"")</f>
+        <f>IF(B15="DIV", F15,"")</f>
         <v/>
       </c>
       <c r="AD45" s="35" t="n"/>
@@ -3297,13 +3210,13 @@
         </is>
       </c>
       <c r="D46" s="26" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E46" s="27" t="n">
-        <v>484.9</v>
+        <v>490.95</v>
       </c>
       <c r="F46" s="27" t="n">
-        <v>969.8099999999999</v>
+        <v>13746.59</v>
       </c>
       <c r="G46" s="25" t="inlineStr">
         <is>
@@ -3311,61 +3224,61 @@
         </is>
       </c>
       <c r="H46" s="26" t="n">
-        <v>0.97</v>
+        <v>13.53</v>
       </c>
       <c r="I46" s="26" t="n">
-        <v>6.94</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="J46" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K46" s="29">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="L46" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="M46" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
         <v/>
       </c>
       <c r="N46" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
         <v/>
       </c>
       <c r="O46" s="29">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="P46" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="Q46" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
         <v/>
       </c>
       <c r="R46" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="S46" s="32">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="T46" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="U46" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
         <v/>
       </c>
       <c r="V46" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="W46" s="33" t="n">
@@ -3375,20 +3288,20 @@
         <v>45806</v>
       </c>
       <c r="Y46" s="37">
-        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="Z46" s="38" t="n">
-        <v>-5659.147</v>
+        <v>-2765.73</v>
       </c>
       <c r="AA46" s="38" t="n">
-        <v>5739.5</v>
+        <v>2805</v>
       </c>
       <c r="AB46" s="39" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC46" s="30">
-        <f>IF(B17="DIV", F17,"")</f>
+        <f>IF(B16="DIV", F16,"")</f>
         <v/>
       </c>
       <c r="AD46" s="35" t="n"/>
@@ -3423,10 +3336,10 @@
         <v>2</v>
       </c>
       <c r="E47" s="27" t="n">
-        <v>485.67</v>
+        <v>484.9</v>
       </c>
       <c r="F47" s="27" t="n">
-        <v>971.33</v>
+        <v>969.8099999999999</v>
       </c>
       <c r="G47" s="25" t="inlineStr">
         <is>
@@ -3437,58 +3350,58 @@
         <v>0.97</v>
       </c>
       <c r="I47" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J47" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K47" s="29">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="L47" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="M47" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
         <v/>
       </c>
       <c r="N47" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
         <v/>
       </c>
       <c r="O47" s="29">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="P47" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="Q47" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
         <v/>
       </c>
       <c r="R47" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="S47" s="32">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="T47" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="U47" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
         <v/>
       </c>
       <c r="V47" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="W47" s="33" t="n">
@@ -3498,20 +3411,20 @@
         <v>45806</v>
       </c>
       <c r="Y47" s="37">
-        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="Z47" s="38" t="n">
-        <v>-2893.6635</v>
+        <v>-5659.147</v>
       </c>
       <c r="AA47" s="38" t="n">
-        <v>2934.75</v>
+        <v>5739.5</v>
       </c>
       <c r="AB47" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC47" s="30">
-        <f>IF(B18="DIV", F18,"")</f>
+        <f>IF(B17="DIV", F17,"")</f>
         <v/>
       </c>
       <c r="AD47" s="35" t="n"/>
@@ -3546,10 +3459,10 @@
         <v>2</v>
       </c>
       <c r="E48" s="27" t="n">
-        <v>485.92</v>
+        <v>485.67</v>
       </c>
       <c r="F48" s="27" t="n">
-        <v>971.83</v>
+        <v>971.33</v>
       </c>
       <c r="G48" s="25" t="inlineStr">
         <is>
@@ -3567,51 +3480,51 @@
         <v/>
       </c>
       <c r="K48" s="29">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="L48" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="M48" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
         <v/>
       </c>
       <c r="N48" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
         <v/>
       </c>
       <c r="O48" s="29">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="P48" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="Q48" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
         <v/>
       </c>
       <c r="R48" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="S48" s="32">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="T48" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="U48" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
         <v/>
       </c>
       <c r="V48" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="W48" s="33" t="n">
@@ -3621,20 +3534,20 @@
         <v>45806</v>
       </c>
       <c r="Y48" s="37">
-        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="Z48" s="38" t="n">
-        <v>-3061.53</v>
+        <v>-2893.6635</v>
       </c>
       <c r="AA48" s="38" t="n">
-        <v>3105</v>
+        <v>2934.75</v>
       </c>
       <c r="AB48" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC48" s="30">
-        <f>IF(B19="DIV", F19,"")</f>
+        <f>IF(B18="DIV", F18,"")</f>
         <v/>
       </c>
       <c r="AD48" s="35" t="n"/>
@@ -3669,10 +3582,10 @@
         <v>2</v>
       </c>
       <c r="E49" s="27" t="n">
-        <v>483.95</v>
+        <v>485.92</v>
       </c>
       <c r="F49" s="27" t="n">
-        <v>967.91</v>
+        <v>971.83</v>
       </c>
       <c r="G49" s="25" t="inlineStr">
         <is>
@@ -3683,58 +3596,58 @@
         <v>0.97</v>
       </c>
       <c r="I49" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J49" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K49" s="29">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="L49" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="M49" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
         <v/>
       </c>
       <c r="N49" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
         <v/>
       </c>
       <c r="O49" s="29">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="P49" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="Q49" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
         <v/>
       </c>
       <c r="R49" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="S49" s="32">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="T49" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="U49" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
         <v/>
       </c>
       <c r="V49" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="W49" s="33" t="n">
@@ -3744,20 +3657,20 @@
         <v>45806</v>
       </c>
       <c r="Y49" s="37">
-        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="Z49" s="38" t="n">
-        <v>-1232.4014</v>
+        <v>-3061.53</v>
       </c>
       <c r="AA49" s="38" t="n">
-        <v>1249.9</v>
+        <v>3105</v>
       </c>
       <c r="AB49" s="39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC49" s="30">
-        <f>IF(B20="DIV", F20,"")</f>
+        <f>IF(B19="DIV", F19,"")</f>
         <v/>
       </c>
       <c r="AD49" s="35" t="n"/>
@@ -3792,10 +3705,10 @@
         <v>2</v>
       </c>
       <c r="E50" s="27" t="n">
-        <v>484.65</v>
+        <v>483.95</v>
       </c>
       <c r="F50" s="27" t="n">
-        <v>969.3099999999999</v>
+        <v>967.91</v>
       </c>
       <c r="G50" s="25" t="inlineStr">
         <is>
@@ -3813,51 +3726,51 @@
         <v/>
       </c>
       <c r="K50" s="29">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="L50" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="M50" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
         <v/>
       </c>
       <c r="N50" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
         <v/>
       </c>
       <c r="O50" s="29">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="P50" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="Q50" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
         <v/>
       </c>
       <c r="R50" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="S50" s="32">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="T50" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="U50" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
         <v/>
       </c>
       <c r="V50" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="W50" s="33" t="n">
@@ -3867,20 +3780,20 @@
         <v>45806</v>
       </c>
       <c r="Y50" s="37">
-        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="Z50" s="38" t="n">
-        <v>-1842.2424</v>
+        <v>-1232.4014</v>
       </c>
       <c r="AA50" s="38" t="n">
-        <v>1868.4</v>
+        <v>1249.9</v>
       </c>
       <c r="AB50" s="39" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC50" s="30">
-        <f>IF(B21="DIV", F21,"")</f>
+        <f>IF(B20="DIV", F20,"")</f>
         <v/>
       </c>
       <c r="AD50" s="35" t="n"/>
@@ -3915,10 +3828,10 @@
         <v>2</v>
       </c>
       <c r="E51" s="27" t="n">
-        <v>486.17</v>
+        <v>484.65</v>
       </c>
       <c r="F51" s="27" t="n">
-        <v>972.33</v>
+        <v>969.3099999999999</v>
       </c>
       <c r="G51" s="25" t="inlineStr">
         <is>
@@ -3929,58 +3842,58 @@
         <v>0.97</v>
       </c>
       <c r="I51" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J51" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K51" s="29">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="L51" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="M51" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
         <v/>
       </c>
       <c r="N51" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
         <v/>
       </c>
       <c r="O51" s="29">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="P51" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="Q51" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
         <v/>
       </c>
       <c r="R51" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="S51" s="32">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="T51" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="U51" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
         <v/>
       </c>
       <c r="V51" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="W51" s="33" t="n">
@@ -3990,20 +3903,20 @@
         <v>45806</v>
       </c>
       <c r="Y51" s="37">
-        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="Z51" s="38" t="n">
-        <v>-648.788</v>
+        <v>-1842.2424</v>
       </c>
       <c r="AA51" s="38" t="n">
-        <v>658</v>
+        <v>1868.4</v>
       </c>
       <c r="AB51" s="39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC51" s="30">
-        <f>IF(B22="DIV", F22,"")</f>
+        <f>IF(B21="DIV", F21,"")</f>
         <v/>
       </c>
       <c r="AD51" s="35" t="n"/>
@@ -4022,7 +3935,7 @@
     </row>
     <row r="52" ht="15.75" customHeight="1" s="62">
       <c r="A52" s="36" t="n">
-        <v>45705</v>
+        <v>45712</v>
       </c>
       <c r="B52" s="25" t="inlineStr">
         <is>
@@ -4035,13 +3948,13 @@
         </is>
       </c>
       <c r="D52" s="26" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E52" s="27" t="n">
-        <v>445.69</v>
+        <v>486.17</v>
       </c>
       <c r="F52" s="27" t="n">
-        <v>8913.73</v>
+        <v>972.33</v>
       </c>
       <c r="G52" s="25" t="inlineStr">
         <is>
@@ -4049,61 +3962,61 @@
         </is>
       </c>
       <c r="H52" s="26" t="n">
-        <v>8.83</v>
+        <v>0.97</v>
       </c>
       <c r="I52" s="26" t="n">
-        <v>63.9</v>
+        <v>6.96</v>
       </c>
       <c r="J52" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K52" s="29">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="L52" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="M52" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
         <v/>
       </c>
       <c r="N52" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
         <v/>
       </c>
       <c r="O52" s="29">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="P52" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="Q52" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
         <v/>
       </c>
       <c r="R52" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="S52" s="32">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="T52" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="U52" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
         <v/>
       </c>
       <c r="V52" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="W52" s="33" t="n">
@@ -4113,20 +4026,20 @@
         <v>45806</v>
       </c>
       <c r="Y52" s="37">
-        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="Z52" s="38" t="n">
-        <v>-1297.4774</v>
+        <v>-648.788</v>
       </c>
       <c r="AA52" s="38" t="n">
-        <v>1315.9</v>
+        <v>658</v>
       </c>
       <c r="AB52" s="39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC52" s="30">
-        <f>IF(B23="DIV", F23,"")</f>
+        <f>IF(B22="DIV", F22,"")</f>
         <v/>
       </c>
       <c r="AD52" s="35" t="n"/>
@@ -4145,7 +4058,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1" s="62">
       <c r="A53" s="36" t="n">
-        <v>45699</v>
+        <v>45705</v>
       </c>
       <c r="B53" s="25" t="inlineStr">
         <is>
@@ -4158,13 +4071,13 @@
         </is>
       </c>
       <c r="D53" s="26" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E53" s="27" t="n">
-        <v>509.46</v>
+        <v>445.69</v>
       </c>
       <c r="F53" s="27" t="n">
-        <v>5094.65</v>
+        <v>8913.73</v>
       </c>
       <c r="G53" s="25" t="inlineStr">
         <is>
@@ -4172,61 +4085,61 @@
         </is>
       </c>
       <c r="H53" s="26" t="n">
-        <v>5.05</v>
+        <v>8.83</v>
       </c>
       <c r="I53" s="26" t="n">
-        <v>36.6</v>
+        <v>63.9</v>
       </c>
       <c r="J53" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K53" s="29">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="L53" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="M53" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
         <v/>
       </c>
       <c r="N53" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
         <v/>
       </c>
       <c r="O53" s="29">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="P53" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="Q53" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
         <v/>
       </c>
       <c r="R53" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="S53" s="32">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="T53" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="U53" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
         <v/>
       </c>
       <c r="V53" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="W53" s="33" t="n">
@@ -4236,20 +4149,20 @@
         <v>45806</v>
       </c>
       <c r="Y53" s="37">
-        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="Z53" s="38" t="n">
-        <v>-1295.604</v>
+        <v>-1297.4774</v>
       </c>
       <c r="AA53" s="38" t="n">
-        <v>1314</v>
+        <v>1315.9</v>
       </c>
       <c r="AB53" s="39" t="n">
         <v>2</v>
       </c>
       <c r="AC53" s="30">
-        <f>IF(B24="DIV", F24,"")</f>
+        <f>IF(B23="DIV", F23,"")</f>
         <v/>
       </c>
       <c r="AD53" s="35" t="n"/>
@@ -4268,7 +4181,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1" s="62">
       <c r="A54" s="36" t="n">
-        <v>45694</v>
+        <v>45699</v>
       </c>
       <c r="B54" s="25" t="inlineStr">
         <is>
@@ -4281,13 +4194,13 @@
         </is>
       </c>
       <c r="D54" s="26" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E54" s="27" t="n">
-        <v>529.3200000000001</v>
+        <v>509.46</v>
       </c>
       <c r="F54" s="27" t="n">
-        <v>10586.46</v>
+        <v>5094.65</v>
       </c>
       <c r="G54" s="25" t="inlineStr">
         <is>
@@ -4295,61 +4208,61 @@
         </is>
       </c>
       <c r="H54" s="26" t="n">
-        <v>10.47</v>
+        <v>5.05</v>
       </c>
       <c r="I54" s="26" t="n">
-        <v>75.98999999999999</v>
+        <v>36.6</v>
       </c>
       <c r="J54" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K54" s="29">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="L54" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
         <v/>
       </c>
       <c r="M54" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
         <v/>
       </c>
       <c r="N54" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
         <v/>
       </c>
       <c r="O54" s="29">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="P54" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
         <v/>
       </c>
       <c r="Q54" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
         <v/>
       </c>
       <c r="R54" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
         <v/>
       </c>
       <c r="S54" s="32">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="T54" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
         <v/>
       </c>
       <c r="U54" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
         <v/>
       </c>
       <c r="V54" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
         <v/>
       </c>
       <c r="W54" s="33" t="n">
@@ -4359,20 +4272,20 @@
         <v>45806</v>
       </c>
       <c r="Y54" s="37">
-        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
         <v/>
       </c>
       <c r="Z54" s="38" t="n">
-        <v>-5624.637</v>
+        <v>-1295.604</v>
       </c>
       <c r="AA54" s="38" t="n">
-        <v>5704.5</v>
+        <v>1314</v>
       </c>
       <c r="AB54" s="39" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AC54" s="30">
-        <f>IF(B25="DIV", F25,"")</f>
+        <f>IF(B24="DIV", F24,"")</f>
         <v/>
       </c>
       <c r="AD54" s="35" t="n"/>
@@ -4390,20 +4303,127 @@
       <c r="AP54" s="40" t="n"/>
     </row>
     <row r="55" ht="15.75" customHeight="1" s="62">
-      <c r="E55" s="41" t="n"/>
-      <c r="F55" s="41" t="n"/>
-      <c r="G55" s="42" t="n"/>
-      <c r="J55" s="41" t="n"/>
-      <c r="K55" s="41" t="n"/>
-      <c r="L55" s="41" t="n"/>
-      <c r="M55" s="1" t="n"/>
-      <c r="W55" s="41" t="n"/>
-      <c r="X55" s="41" t="n"/>
-      <c r="Y55" s="41" t="n"/>
-      <c r="Z55" s="41" t="n"/>
-      <c r="AA55" s="41" t="n"/>
-      <c r="AB55" s="41" t="n"/>
-      <c r="AC55" s="41" t="n"/>
+      <c r="A55" s="36" t="n">
+        <v>45694</v>
+      </c>
+      <c r="B55" s="25" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C55" s="25" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D55" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="E55" s="27" t="n">
+        <v>529.3200000000001</v>
+      </c>
+      <c r="F55" s="27" t="n">
+        <v>10586.46</v>
+      </c>
+      <c r="G55" s="25" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H55" s="26" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="I55" s="26" t="n">
+        <v>75.98999999999999</v>
+      </c>
+      <c r="J55" s="28">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K55" s="29">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="L55" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="M55" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <v/>
+      </c>
+      <c r="N55" s="31">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <v/>
+      </c>
+      <c r="O55" s="29">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="P55" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="Q55" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <v/>
+      </c>
+      <c r="R55" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <v/>
+      </c>
+      <c r="S55" s="32">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="T55" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="U55" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <v/>
+      </c>
+      <c r="V55" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <v/>
+      </c>
+      <c r="W55" s="33" t="n">
+        <v>703.9400000000001</v>
+      </c>
+      <c r="X55" s="36" t="n">
+        <v>45806</v>
+      </c>
+      <c r="Y55" s="37">
+        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="Z55" s="38" t="n">
+        <v>-5624.637</v>
+      </c>
+      <c r="AA55" s="38" t="n">
+        <v>5704.5</v>
+      </c>
+      <c r="AB55" s="39" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC55" s="30">
+        <f>IF(B25="DIV", F25,"")</f>
+        <v/>
+      </c>
+      <c r="AD55" s="35" t="n"/>
+      <c r="AE55" s="40" t="n"/>
+      <c r="AF55" s="40" t="n"/>
+      <c r="AG55" s="40" t="n"/>
+      <c r="AH55" s="40" t="n"/>
+      <c r="AI55" s="40" t="n"/>
+      <c r="AJ55" s="40" t="n"/>
+      <c r="AK55" s="40" t="n"/>
+      <c r="AL55" s="40" t="n"/>
+      <c r="AM55" s="40" t="n"/>
+      <c r="AN55" s="40" t="n"/>
+      <c r="AO55" s="40" t="n"/>
+      <c r="AP55" s="40" t="n"/>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="62">
       <c r="E56" s="41" t="n"/>
@@ -19372,6 +19392,7 @@
       <c r="J991" s="41" t="n"/>
       <c r="K991" s="41" t="n"/>
       <c r="L991" s="41" t="n"/>
+      <c r="M991" s="1" t="n"/>
       <c r="W991" s="41" t="n"/>
       <c r="X991" s="41" t="n"/>
       <c r="Y991" s="41" t="n"/>
@@ -19619,6 +19640,21 @@
       <c r="AA1007" s="41" t="n"/>
       <c r="AB1007" s="41" t="n"/>
       <c r="AC1007" s="41" t="n"/>
+    </row>
+    <row r="1008">
+      <c r="E1008" s="41" t="n"/>
+      <c r="F1008" s="41" t="n"/>
+      <c r="G1008" s="42" t="n"/>
+      <c r="J1008" s="41" t="n"/>
+      <c r="K1008" s="41" t="n"/>
+      <c r="L1008" s="41" t="n"/>
+      <c r="W1008" s="41" t="n"/>
+      <c r="X1008" s="41" t="n"/>
+      <c r="Y1008" s="41" t="n"/>
+      <c r="Z1008" s="41" t="n"/>
+      <c r="AA1008" s="41" t="n"/>
+      <c r="AB1008" s="41" t="n"/>
+      <c r="AC1008" s="41" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:AO53"/>

</xml_diff>

<commit_message>
Update stock data files - final batch
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/High Energy Batteries (India) Ltd.xlsx
+++ b/dumps/Stocks/High Energy Batteries (India) Ltd.xlsx
@@ -712,7 +712,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1008"/>
+  <dimension ref="A1:AP1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G19" activePane="bottomRight" state="frozen"/>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" s="62">
       <c r="A5" s="73" t="n">
-        <v>45978</v>
+        <v>45982</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1078,18 +1078,18 @@
         <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>657.58</v>
+        <v>621</v>
       </c>
       <c r="F5" t="n">
-        <v>3304.35</v>
+        <v>3120.55</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CN#252608260909</t>
+          <t>CN#252608495287</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>16.45</v>
+        <v>15.55</v>
       </c>
       <c r="J5">
         <f>Index!$C$2</f>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" s="62">
       <c r="A6" s="73" t="n">
-        <v>45967</v>
+        <v>45979</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1111,21 +1111,21 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>570.45</v>
+        <v>623.66</v>
       </c>
       <c r="F6" t="n">
-        <v>5733</v>
+        <v>3133.87</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>CN#252607785263</t>
+          <t>CN#252608322011</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>28.5</v>
+        <v>15.57</v>
       </c>
       <c r="J6">
         <f>Index!$C$2</f>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" s="62">
       <c r="A7" s="73" t="n">
-        <v>45961</v>
+        <v>45978</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1150,18 +1150,18 @@
         <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>596.15</v>
+        <v>657.58</v>
       </c>
       <c r="F7" t="n">
-        <v>2995.65</v>
+        <v>3304.35</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>CN#252607606298</t>
+          <t>CN#252608260909</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>14.9</v>
+        <v>16.45</v>
       </c>
       <c r="J7">
         <f>Index!$C$2</f>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="8" ht="15.75" customHeight="1" s="62">
       <c r="A8" s="73" t="n">
-        <v>45957</v>
+        <v>45967</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1186,18 +1186,18 @@
         <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>607.4</v>
+        <v>570.45</v>
       </c>
       <c r="F8" t="n">
-        <v>6104.4</v>
+        <v>5733</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CN#252607382790</t>
+          <t>CN#252607785263</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>30.4</v>
+        <v>28.5</v>
       </c>
       <c r="J8">
         <f>Index!$C$2</f>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1" s="62">
       <c r="A9" s="73" t="n">
-        <v>46063</v>
+        <v>45961</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1219,24 +1219,21 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E9" t="n">
-        <v>589.75</v>
+        <v>596.15</v>
       </c>
       <c r="F9" t="n">
-        <v>5946.05</v>
+        <v>2995.65</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>CN#252611730667</t>
+          <t>CN#252607606298</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>5.89</v>
-      </c>
       <c r="I9" t="n">
-        <v>42.66</v>
+        <v>14.9</v>
       </c>
       <c r="J9">
         <f>Index!$C$2</f>
@@ -1244,8 +1241,8 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="62">
-      <c r="A10" s="60" t="n">
-        <v>46050</v>
+      <c r="A10" s="73" t="n">
+        <v>45957</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1261,26 +1258,27 @@
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>530</v>
+        <v>607.4</v>
       </c>
       <c r="F10" t="n">
-        <v>5343.69</v>
+        <v>6104.4</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>CN#252607382790</t>
         </is>
       </c>
-      <c r="H10" t="n">
-        <v>5.33</v>
-      </c>
       <c r="I10" t="n">
-        <v>38.36</v>
+        <v>30.4</v>
+      </c>
+      <c r="J10">
+        <f>Index!$C$2</f>
+        <v/>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="62">
-      <c r="A11" s="60" t="n">
-        <v>46049</v>
+      <c r="A11" s="73" t="n">
+        <v>46063</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1293,29 +1291,33 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>534.7</v>
+        <v>589.75</v>
       </c>
       <c r="F11" t="n">
-        <v>2695.48</v>
+        <v>5946.05</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>CN#252611730667</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>2.67</v>
+        <v>5.89</v>
       </c>
       <c r="I11" t="n">
-        <v>19.31</v>
+        <v>42.66</v>
+      </c>
+      <c r="J11">
+        <f>Index!$C$2</f>
+        <v/>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="62">
       <c r="A12" s="60" t="n">
-        <v>46042</v>
+        <v>46050</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1331,10 +1333,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="n">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="F12" t="n">
-        <v>5454.64</v>
+        <v>5343.69</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1342,15 +1344,15 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>5.42</v>
+        <v>5.33</v>
       </c>
       <c r="I12" t="n">
-        <v>39.22</v>
+        <v>38.36</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="62">
       <c r="A13" s="60" t="n">
-        <v>46030</v>
+        <v>46049</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1363,13 +1365,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>563.85</v>
+        <v>534.7</v>
       </c>
       <c r="F13" t="n">
-        <v>5684.91</v>
+        <v>2695.48</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1377,15 +1379,15 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>5.62</v>
+        <v>2.67</v>
       </c>
       <c r="I13" t="n">
-        <v>40.79</v>
+        <v>19.31</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="62">
       <c r="A14" s="60" t="n">
-        <v>46017</v>
+        <v>46042</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1398,13 +1400,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>545.55</v>
+        <v>541</v>
       </c>
       <c r="F14" t="n">
-        <v>2750.24</v>
+        <v>5454.64</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1412,15 +1414,15 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>2.74</v>
+        <v>5.42</v>
       </c>
       <c r="I14" t="n">
-        <v>19.75</v>
+        <v>39.22</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="62">
       <c r="A15" s="60" t="n">
-        <v>46017</v>
+        <v>46030</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1433,13 +1435,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
-        <v>545.5</v>
+        <v>563.85</v>
       </c>
       <c r="F15" t="n">
-        <v>2749.99</v>
+        <v>5684.91</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1447,15 +1449,15 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>2.74</v>
+        <v>5.62</v>
       </c>
       <c r="I15" t="n">
-        <v>19.75</v>
+        <v>40.79</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="62">
       <c r="A16" s="60" t="n">
-        <v>46015</v>
+        <v>46017</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1468,13 +1470,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E16" t="n">
-        <v>545.25</v>
+        <v>545.55</v>
       </c>
       <c r="F16" t="n">
-        <v>5497.42</v>
+        <v>2750.24</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1482,15 +1484,15 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>5.42</v>
+        <v>2.74</v>
       </c>
       <c r="I16" t="n">
-        <v>39.5</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="62">
       <c r="A17" s="60" t="n">
-        <v>46014</v>
+        <v>46017</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1503,13 +1505,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E17" t="n">
-        <v>548.9</v>
+        <v>545.5</v>
       </c>
       <c r="F17" t="n">
-        <v>5534.11</v>
+        <v>2749.99</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -1517,15 +1519,15 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>5.47</v>
+        <v>2.74</v>
       </c>
       <c r="I17" t="n">
-        <v>39.64</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="62">
       <c r="A18" s="60" t="n">
-        <v>46007</v>
+        <v>46015</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1541,10 +1543,10 @@
         <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>541.3</v>
+        <v>545.25</v>
       </c>
       <c r="F18" t="n">
-        <v>5457.59</v>
+        <v>5497.42</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -1552,15 +1554,15 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>5.39</v>
+        <v>5.42</v>
       </c>
       <c r="I18" t="n">
-        <v>39.2</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="62">
       <c r="A19" s="60" t="n">
-        <v>46002</v>
+        <v>46014</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1573,13 +1575,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E19" t="n">
-        <v>547.9</v>
+        <v>548.9</v>
       </c>
       <c r="F19" t="n">
-        <v>2762.01</v>
+        <v>5534.11</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1587,15 +1589,15 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>2.75</v>
+        <v>5.47</v>
       </c>
       <c r="I19" t="n">
-        <v>19.76</v>
+        <v>39.64</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="62">
       <c r="A20" s="60" t="n">
-        <v>46000</v>
+        <v>46007</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1608,13 +1610,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>560.95</v>
+        <v>541.3</v>
       </c>
       <c r="F20" t="n">
-        <v>2827.8</v>
+        <v>5457.59</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1622,15 +1624,15 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>2.8</v>
+        <v>5.39</v>
       </c>
       <c r="I20" t="n">
-        <v>20.25</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="62">
       <c r="A21" s="60" t="n">
-        <v>46000</v>
+        <v>46002</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1646,10 +1648,10 @@
         <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>561</v>
+        <v>547.9</v>
       </c>
       <c r="F21" t="n">
-        <v>2828.11</v>
+        <v>2762.01</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1657,15 +1659,15 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>2.8</v>
+        <v>2.75</v>
       </c>
       <c r="I21" t="n">
-        <v>20.31</v>
+        <v>19.76</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="62">
       <c r="A22" s="60" t="n">
-        <v>45996</v>
+        <v>46000</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1678,13 +1680,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>573.95</v>
+        <v>560.95</v>
       </c>
       <c r="F22" t="n">
-        <v>5786.76</v>
+        <v>2827.8</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1692,15 +1694,15 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>5.72</v>
+        <v>2.8</v>
       </c>
       <c r="I22" t="n">
-        <v>41.54</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="62">
       <c r="A23" s="60" t="n">
-        <v>45989</v>
+        <v>46000</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1716,10 +1718,10 @@
         <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>586.95</v>
+        <v>561</v>
       </c>
       <c r="F23" t="n">
-        <v>2958.88</v>
+        <v>2828.11</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1727,15 +1729,15 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>2.93</v>
+        <v>2.8</v>
       </c>
       <c r="I23" t="n">
-        <v>21.2</v>
+        <v>20.31</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="62">
       <c r="A24" s="60" t="n">
-        <v>45982</v>
+        <v>45996</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1748,13 +1750,13 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E24" t="n">
-        <v>621</v>
+        <v>573.95</v>
       </c>
       <c r="F24" t="n">
-        <v>3130.59</v>
+        <v>5786.76</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1762,15 +1764,15 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>3.11</v>
+        <v>5.72</v>
       </c>
       <c r="I24" t="n">
-        <v>22.48</v>
+        <v>41.54</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="62">
       <c r="A25" s="60" t="n">
-        <v>45979</v>
+        <v>45989</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1783,13 +1785,13 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E25" t="n">
-        <v>624.95</v>
+        <v>586.95</v>
       </c>
       <c r="F25" t="n">
-        <v>1260.17</v>
+        <v>2958.88</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1797,15 +1799,15 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>1.25</v>
+        <v>2.93</v>
       </c>
       <c r="I25" t="n">
-        <v>9.02</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="62">
       <c r="A26" s="60" t="n">
-        <v>45979</v>
+        <v>45982</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1818,13 +1820,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E26" t="n">
-        <v>622.8</v>
+        <v>621</v>
       </c>
       <c r="F26" t="n">
-        <v>1883.78</v>
+        <v>3130.59</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1832,15 +1834,15 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>1.88</v>
+        <v>3.11</v>
       </c>
       <c r="I26" t="n">
-        <v>13.5</v>
+        <v>22.48</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="62">
       <c r="A27" s="60" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1853,13 +1855,13 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" t="n">
-        <v>658</v>
+        <v>624.95</v>
       </c>
       <c r="F27" t="n">
-        <v>663.4299999999999</v>
+        <v>1260.17</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1867,15 +1869,15 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>0.66</v>
+        <v>1.25</v>
       </c>
       <c r="I27" t="n">
-        <v>4.77</v>
+        <v>9.02</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="62">
       <c r="A28" s="60" t="n">
-        <v>45978</v>
+        <v>45979</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1888,13 +1890,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" t="n">
-        <v>657.95</v>
+        <v>622.8</v>
       </c>
       <c r="F28" t="n">
-        <v>1326.73</v>
+        <v>1883.78</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1902,10 +1904,10 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>1.32</v>
+        <v>1.88</v>
       </c>
       <c r="I28" t="n">
-        <v>9.51</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="62">
@@ -1923,13 +1925,13 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F29" t="n">
-        <v>1324.82</v>
+        <v>663.4299999999999</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1937,15 +1939,15 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>1.32</v>
+        <v>0.66</v>
       </c>
       <c r="I29" t="n">
-        <v>9.5</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="62">
       <c r="A30" s="60" t="n">
-        <v>45967</v>
+        <v>45978</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1958,13 +1960,13 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E30" t="n">
-        <v>570.45</v>
+        <v>657.95</v>
       </c>
       <c r="F30" t="n">
-        <v>5751.49</v>
+        <v>1326.73</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1972,15 +1974,15 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>5.74</v>
+        <v>1.32</v>
       </c>
       <c r="I30" t="n">
-        <v>41.25</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="62">
       <c r="A31" s="60" t="n">
-        <v>45961</v>
+        <v>45978</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1993,13 +1995,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E31" t="n">
-        <v>596.15</v>
+        <v>657</v>
       </c>
       <c r="F31" t="n">
-        <v>3005.27</v>
+        <v>1324.82</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -2007,15 +2009,15 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>2.97</v>
+        <v>1.32</v>
       </c>
       <c r="I31" t="n">
-        <v>21.55</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="62">
       <c r="A32" s="60" t="n">
-        <v>45957</v>
+        <v>45967</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2031,10 +2033,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="n">
-        <v>607.4</v>
+        <v>570.45</v>
       </c>
       <c r="F32" t="n">
-        <v>6124.02</v>
+        <v>5751.49</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -2042,15 +2044,15 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>6.08</v>
+        <v>5.74</v>
       </c>
       <c r="I32" t="n">
-        <v>43.94</v>
+        <v>41.25</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="62">
       <c r="A33" s="60" t="n">
-        <v>45954</v>
+        <v>45961</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2066,10 +2068,10 @@
         <v>5</v>
       </c>
       <c r="E33" t="n">
-        <v>647.9</v>
+        <v>596.15</v>
       </c>
       <c r="F33" t="n">
-        <v>3266.17</v>
+        <v>3005.27</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -2077,15 +2079,15 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>3.24</v>
+        <v>2.97</v>
       </c>
       <c r="I33" t="n">
-        <v>23.43</v>
+        <v>21.55</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="62">
       <c r="A34" s="60" t="n">
-        <v>45953</v>
+        <v>45957</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2101,10 +2103,10 @@
         <v>10</v>
       </c>
       <c r="E34" t="n">
-        <v>651.4</v>
+        <v>607.4</v>
       </c>
       <c r="F34" t="n">
-        <v>6567.59</v>
+        <v>6124.02</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -2112,15 +2114,15 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>6.49</v>
+        <v>6.08</v>
       </c>
       <c r="I34" t="n">
-        <v>47.1</v>
+        <v>43.94</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="62">
       <c r="A35" s="60" t="n">
-        <v>45950</v>
+        <v>45954</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2133,13 +2135,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E35" t="n">
-        <v>640.95</v>
+        <v>647.9</v>
       </c>
       <c r="F35" t="n">
-        <v>6462.21</v>
+        <v>3266.17</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -2147,15 +2149,15 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>6.4</v>
+        <v>3.24</v>
       </c>
       <c r="I35" t="n">
-        <v>46.31</v>
+        <v>23.43</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="62">
       <c r="A36" s="60" t="n">
-        <v>45947</v>
+        <v>45953</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -2171,10 +2173,10 @@
         <v>10</v>
       </c>
       <c r="E36" t="n">
-        <v>610.5</v>
+        <v>651.4</v>
       </c>
       <c r="F36" t="n">
-        <v>6155.25</v>
+        <v>6567.59</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
@@ -2182,211 +2184,85 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>6.12</v>
+        <v>6.49</v>
       </c>
       <c r="I36" t="n">
-        <v>44.13</v>
+        <v>47.1</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1" s="62">
-      <c r="A37" s="36" t="n">
-        <v>45807</v>
-      </c>
-      <c r="B37" s="25" t="inlineStr">
+      <c r="A37" s="60" t="n">
+        <v>45950</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>BSE</t>
         </is>
       </c>
-      <c r="C37" s="25" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
-      <c r="D37" s="26" t="n">
-        <v>50</v>
-      </c>
-      <c r="E37" s="27" t="n">
-        <v>714.28</v>
-      </c>
-      <c r="F37" s="27">
-        <f>D7*E7</f>
-        <v/>
-      </c>
-      <c r="G37" s="25" t="inlineStr">
+      <c r="D37" t="n">
+        <v>10</v>
+      </c>
+      <c r="E37" t="n">
+        <v>640.95</v>
+      </c>
+      <c r="F37" t="n">
+        <v>6462.21</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H37" s="26" t="n"/>
-      <c r="I37" s="26" t="n"/>
-      <c r="J37" s="28">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K37" s="29">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="L37" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="M37" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
-        <v/>
-      </c>
-      <c r="N37" s="31">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
-        <v/>
-      </c>
-      <c r="O37" s="29">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="P37" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="Q37" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
-        <v/>
-      </c>
-      <c r="R37" s="30">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
-        <v/>
-      </c>
-      <c r="S37" s="32">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="T37" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
-        <v/>
-      </c>
-      <c r="U37" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
-        <v/>
-      </c>
-      <c r="V37" s="33">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
-        <v/>
-      </c>
-      <c r="W37" s="33" t="n"/>
-      <c r="X37" s="33" t="n"/>
-      <c r="Y37" s="32">
-        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/SUM(F7:I7), "")</f>
-        <v/>
-      </c>
-      <c r="Z37" s="33" t="n"/>
-      <c r="AA37" s="33" t="n"/>
-      <c r="AB37" s="34" t="n"/>
-      <c r="AC37" s="30">
-        <f>IF(B7="DIV", F7,"")</f>
-        <v/>
-      </c>
-      <c r="AD37" s="35" t="n"/>
+      <c r="H37" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="I37" t="n">
+        <v>46.31</v>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1" s="62">
-      <c r="A38" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="B38" s="25" t="inlineStr">
+      <c r="A38" s="60" t="n">
+        <v>45947</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>BSE</t>
         </is>
       </c>
-      <c r="C38" s="25" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
-      <c r="D38" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="E38" s="27" t="n">
-        <v>699.39</v>
-      </c>
-      <c r="F38" s="27">
-        <f>D8*E8</f>
-        <v/>
-      </c>
-      <c r="G38" s="25" t="inlineStr">
+      <c r="D38" t="n">
+        <v>10</v>
+      </c>
+      <c r="E38" t="n">
+        <v>610.5</v>
+      </c>
+      <c r="F38" t="n">
+        <v>6155.25</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H38" s="26" t="n"/>
-      <c r="I38" s="26" t="n"/>
-      <c r="J38" s="28">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K38" s="29">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="L38" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
-        <v/>
-      </c>
-      <c r="M38" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
-        <v/>
-      </c>
-      <c r="N38" s="31">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
-        <v/>
-      </c>
-      <c r="O38" s="29">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="P38" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
-        <v/>
-      </c>
-      <c r="Q38" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
-        <v/>
-      </c>
-      <c r="R38" s="30">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
-        <v/>
-      </c>
-      <c r="S38" s="32">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="T38" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
-        <v/>
-      </c>
-      <c r="U38" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
-        <v/>
-      </c>
-      <c r="V38" s="33">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
-        <v/>
-      </c>
-      <c r="W38" s="33" t="n"/>
-      <c r="X38" s="33" t="n"/>
-      <c r="Y38" s="32">
-        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/SUM(F8:I8), "")</f>
-        <v/>
-      </c>
-      <c r="Z38" s="33" t="n"/>
-      <c r="AA38" s="33" t="n"/>
-      <c r="AB38" s="34" t="n"/>
-      <c r="AC38" s="30">
-        <f>IF(B8="DIV", F8,"")</f>
-        <v/>
-      </c>
-      <c r="AD38" s="35" t="n"/>
+      <c r="H38" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="I38" t="n">
+        <v>44.13</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1" s="62">
       <c r="A39" s="36" t="n">
-        <v>45806</v>
+        <v>45807</v>
       </c>
       <c r="B39" s="25" t="inlineStr">
         <is>
@@ -2399,13 +2275,13 @@
         </is>
       </c>
       <c r="D39" s="26" t="n">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E39" s="27" t="n">
-        <v>702.78</v>
+        <v>714.28</v>
       </c>
       <c r="F39" s="27">
-        <f>D9*E9</f>
+        <f>D7*E7</f>
         <v/>
       </c>
       <c r="G39" s="25" t="inlineStr">
@@ -2420,64 +2296,64 @@
         <v/>
       </c>
       <c r="K39" s="29">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="L39" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="M39" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
         <v/>
       </c>
       <c r="N39" s="31">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
         <v/>
       </c>
       <c r="O39" s="29">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="P39" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="Q39" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
         <v/>
       </c>
       <c r="R39" s="30">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="S39" s="32">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="T39" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="U39" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
         <v/>
       </c>
       <c r="V39" s="33">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="W39" s="33" t="n"/>
       <c r="X39" s="33" t="n"/>
       <c r="Y39" s="32">
-        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/SUM(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/SUM(F7:I7), "")</f>
         <v/>
       </c>
       <c r="Z39" s="33" t="n"/>
       <c r="AA39" s="33" t="n"/>
       <c r="AB39" s="34" t="n"/>
       <c r="AC39" s="30">
-        <f>IF(B9="DIV", F9,"")</f>
+        <f>IF(B7="DIV", F7,"")</f>
         <v/>
       </c>
       <c r="AD39" s="35" t="n"/>
@@ -2497,13 +2373,13 @@
         </is>
       </c>
       <c r="D40" s="26" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E40" s="27" t="n">
-        <v>699.29</v>
+        <v>699.39</v>
       </c>
       <c r="F40" s="27">
-        <f>D10*E10</f>
+        <f>D8*E8</f>
         <v/>
       </c>
       <c r="G40" s="25" t="inlineStr">
@@ -2518,71 +2394,71 @@
         <v/>
       </c>
       <c r="K40" s="29">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="L40" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="M40" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
         <v/>
       </c>
       <c r="N40" s="31">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
         <v/>
       </c>
       <c r="O40" s="29">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="P40" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="Q40" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
         <v/>
       </c>
       <c r="R40" s="30">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="S40" s="32">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="T40" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="U40" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
         <v/>
       </c>
       <c r="V40" s="33">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="W40" s="33" t="n"/>
       <c r="X40" s="33" t="n"/>
       <c r="Y40" s="32">
-        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/SUM(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/SUM(F8:I8), "")</f>
         <v/>
       </c>
       <c r="Z40" s="33" t="n"/>
       <c r="AA40" s="33" t="n"/>
       <c r="AB40" s="34" t="n"/>
       <c r="AC40" s="30">
-        <f>IF(B10="DIV", F10,"")</f>
+        <f>IF(B8="DIV", F8,"")</f>
         <v/>
       </c>
       <c r="AD40" s="35" t="n"/>
     </row>
     <row r="41" ht="15.75" customHeight="1" s="62">
       <c r="A41" s="36" t="n">
-        <v>45712</v>
+        <v>45806</v>
       </c>
       <c r="B41" s="25" t="inlineStr">
         <is>
@@ -2591,121 +2467,96 @@
       </c>
       <c r="C41" s="25" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="D41" s="26" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E41" s="27" t="n">
-        <v>484.4</v>
-      </c>
-      <c r="F41" s="27" t="n">
-        <v>968.8099999999999</v>
+        <v>702.78</v>
+      </c>
+      <c r="F41" s="27">
+        <f>D9*E9</f>
+        <v/>
       </c>
       <c r="G41" s="25" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H41" s="26" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="I41" s="26" t="n">
-        <v>6.94</v>
-      </c>
+      <c r="H41" s="26" t="n"/>
+      <c r="I41" s="26" t="n"/>
       <c r="J41" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K41" s="29">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="L41" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="M41" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
         <v/>
       </c>
       <c r="N41" s="31">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
         <v/>
       </c>
       <c r="O41" s="29">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="P41" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="Q41" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
         <v/>
       </c>
       <c r="R41" s="30">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
         <v/>
       </c>
       <c r="S41" s="32">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/SUM(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/SUM(F9:I9), "")</f>
         <v/>
       </c>
       <c r="T41" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="U41" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
         <v/>
       </c>
       <c r="V41" s="33">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
-        <v/>
-      </c>
-      <c r="W41" s="33" t="n">
-        <v>703.9400000000001</v>
-      </c>
-      <c r="X41" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="Y41" s="37">
-        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/SUM(F11:I11), "")</f>
-        <v/>
-      </c>
-      <c r="Z41" s="38" t="n">
-        <v>-5376.165</v>
-      </c>
-      <c r="AA41" s="38" t="n">
-        <v>5452.5</v>
-      </c>
-      <c r="AB41" s="39" t="n">
-        <v>10</v>
-      </c>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <v/>
+      </c>
+      <c r="W41" s="33" t="n"/>
+      <c r="X41" s="33" t="n"/>
+      <c r="Y41" s="32">
+        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/SUM(F9:I9), "")</f>
+        <v/>
+      </c>
+      <c r="Z41" s="33" t="n"/>
+      <c r="AA41" s="33" t="n"/>
+      <c r="AB41" s="34" t="n"/>
       <c r="AC41" s="30">
-        <f>IF(B11="DIV", F11,"")</f>
+        <f>IF(B9="DIV", F9,"")</f>
         <v/>
       </c>
       <c r="AD41" s="35" t="n"/>
-      <c r="AE41" s="40" t="n"/>
-      <c r="AF41" s="40" t="n"/>
-      <c r="AG41" s="40" t="n"/>
-      <c r="AH41" s="40" t="n"/>
-      <c r="AI41" s="40" t="n"/>
-      <c r="AJ41" s="40" t="n"/>
-      <c r="AK41" s="40" t="n"/>
-      <c r="AL41" s="40" t="n"/>
-      <c r="AM41" s="40" t="n"/>
-      <c r="AN41" s="40" t="n"/>
-      <c r="AO41" s="40" t="n"/>
-      <c r="AP41" s="40" t="n"/>
     </row>
     <row r="42" ht="15.75" customHeight="1" s="62">
       <c r="A42" s="36" t="n">
-        <v>45712</v>
+        <v>45806</v>
       </c>
       <c r="B42" s="25" t="inlineStr">
         <is>
@@ -2714,117 +2565,92 @@
       </c>
       <c r="C42" s="25" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="D42" s="26" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E42" s="27" t="n">
-        <v>486.42</v>
-      </c>
-      <c r="F42" s="27" t="n">
-        <v>972.83</v>
+        <v>699.29</v>
+      </c>
+      <c r="F42" s="27">
+        <f>D10*E10</f>
+        <v/>
       </c>
       <c r="G42" s="25" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H42" s="26" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="I42" s="26" t="n">
-        <v>6.96</v>
-      </c>
+      <c r="H42" s="26" t="n"/>
+      <c r="I42" s="26" t="n"/>
       <c r="J42" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K42" s="29">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="L42" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="M42" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
         <v/>
       </c>
       <c r="N42" s="31">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
         <v/>
       </c>
       <c r="O42" s="29">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="P42" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="Q42" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
         <v/>
       </c>
       <c r="R42" s="30">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
         <v/>
       </c>
       <c r="S42" s="32">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/SUM(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/SUM(F10:I10), "")</f>
         <v/>
       </c>
       <c r="T42" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="U42" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
         <v/>
       </c>
       <c r="V42" s="33">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
-        <v/>
-      </c>
-      <c r="W42" s="33" t="n">
-        <v>703.9400000000001</v>
-      </c>
-      <c r="X42" s="36" t="n">
-        <v>45806</v>
-      </c>
-      <c r="Y42" s="37">
-        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/SUM(F12:I12), "")</f>
-        <v/>
-      </c>
-      <c r="Z42" s="38" t="n">
-        <v>-5412.154</v>
-      </c>
-      <c r="AA42" s="38" t="n">
-        <v>5489</v>
-      </c>
-      <c r="AB42" s="39" t="n">
-        <v>10</v>
-      </c>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <v/>
+      </c>
+      <c r="W42" s="33" t="n"/>
+      <c r="X42" s="33" t="n"/>
+      <c r="Y42" s="32">
+        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/SUM(F10:I10), "")</f>
+        <v/>
+      </c>
+      <c r="Z42" s="33" t="n"/>
+      <c r="AA42" s="33" t="n"/>
+      <c r="AB42" s="34" t="n"/>
       <c r="AC42" s="30">
-        <f>IF(B12="DIV", F12,"")</f>
+        <f>IF(B10="DIV", F10,"")</f>
         <v/>
       </c>
       <c r="AD42" s="35" t="n"/>
-      <c r="AE42" s="40" t="n"/>
-      <c r="AF42" s="40" t="n"/>
-      <c r="AG42" s="40" t="n"/>
-      <c r="AH42" s="40" t="n"/>
-      <c r="AI42" s="40" t="n"/>
-      <c r="AJ42" s="40" t="n"/>
-      <c r="AK42" s="40" t="n"/>
-      <c r="AL42" s="40" t="n"/>
-      <c r="AM42" s="40" t="n"/>
-      <c r="AN42" s="40" t="n"/>
-      <c r="AO42" s="40" t="n"/>
-      <c r="AP42" s="40" t="n"/>
     </row>
     <row r="43" ht="15.75" customHeight="1" s="62">
       <c r="A43" s="36" t="n">
@@ -2844,10 +2670,10 @@
         <v>2</v>
       </c>
       <c r="E43" s="27" t="n">
-        <v>485.17</v>
+        <v>484.4</v>
       </c>
       <c r="F43" s="27" t="n">
-        <v>970.33</v>
+        <v>968.8099999999999</v>
       </c>
       <c r="G43" s="25" t="inlineStr">
         <is>
@@ -2858,58 +2684,58 @@
         <v>0.97</v>
       </c>
       <c r="I43" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J43" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K43" s="29">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="L43" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="M43" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
         <v/>
       </c>
       <c r="N43" s="31">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
         <v/>
       </c>
       <c r="O43" s="29">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="P43" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="Q43" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
         <v/>
       </c>
       <c r="R43" s="30">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="S43" s="32">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="T43" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="U43" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
         <v/>
       </c>
       <c r="V43" s="33">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="W43" s="33" t="n">
@@ -2919,20 +2745,20 @@
         <v>45806</v>
       </c>
       <c r="Y43" s="37">
-        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/SUM(F11:I11), "")</f>
         <v/>
       </c>
       <c r="Z43" s="38" t="n">
-        <v>-5337.218</v>
+        <v>-5376.165</v>
       </c>
       <c r="AA43" s="38" t="n">
-        <v>5413</v>
+        <v>5452.5</v>
       </c>
       <c r="AB43" s="39" t="n">
         <v>10</v>
       </c>
       <c r="AC43" s="30">
-        <f>IF(B13="DIV", F13,"")</f>
+        <f>IF(B11="DIV", F11,"")</f>
         <v/>
       </c>
       <c r="AD43" s="35" t="n"/>
@@ -2967,10 +2793,10 @@
         <v>2</v>
       </c>
       <c r="E44" s="27" t="n">
-        <v>485.42</v>
+        <v>486.42</v>
       </c>
       <c r="F44" s="27" t="n">
-        <v>970.83</v>
+        <v>972.83</v>
       </c>
       <c r="G44" s="25" t="inlineStr">
         <is>
@@ -2988,51 +2814,51 @@
         <v/>
       </c>
       <c r="K44" s="29">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="L44" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="M44" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
         <v/>
       </c>
       <c r="N44" s="31">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
         <v/>
       </c>
       <c r="O44" s="29">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="P44" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="Q44" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
         <v/>
       </c>
       <c r="R44" s="30">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="S44" s="32">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="T44" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="U44" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
         <v/>
       </c>
       <c r="V44" s="33">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="W44" s="33" t="n">
@@ -3042,20 +2868,20 @@
         <v>45806</v>
       </c>
       <c r="Y44" s="37">
-        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/SUM(F12:I12), "")</f>
         <v/>
       </c>
       <c r="Z44" s="38" t="n">
-        <v>-2701.147</v>
+        <v>-5412.154</v>
       </c>
       <c r="AA44" s="38" t="n">
-        <v>2739.5</v>
+        <v>5489</v>
       </c>
       <c r="AB44" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC44" s="30">
-        <f>IF(B14="DIV", F14,"")</f>
+        <f>IF(B12="DIV", F12,"")</f>
         <v/>
       </c>
       <c r="AD44" s="35" t="n"/>
@@ -3090,10 +2916,10 @@
         <v>2</v>
       </c>
       <c r="E45" s="27" t="n">
-        <v>484.15</v>
+        <v>485.17</v>
       </c>
       <c r="F45" s="27" t="n">
-        <v>968.3099999999999</v>
+        <v>970.33</v>
       </c>
       <c r="G45" s="25" t="inlineStr">
         <is>
@@ -3104,58 +2930,58 @@
         <v>0.97</v>
       </c>
       <c r="I45" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J45" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K45" s="29">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="L45" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="M45" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
         <v/>
       </c>
       <c r="N45" s="31">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
         <v/>
       </c>
       <c r="O45" s="29">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="P45" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="Q45" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
         <v/>
       </c>
       <c r="R45" s="30">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="S45" s="32">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="T45" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
         <v/>
       </c>
       <c r="U45" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
         <v/>
       </c>
       <c r="V45" s="33">
-        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
         <v/>
       </c>
       <c r="W45" s="33" t="n">
@@ -3165,20 +2991,20 @@
         <v>45806</v>
       </c>
       <c r="Y45" s="37">
-        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
+        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/SUM(F13:I13), "")</f>
         <v/>
       </c>
       <c r="Z45" s="38" t="n">
-        <v>-2765.4835</v>
+        <v>-5337.218</v>
       </c>
       <c r="AA45" s="38" t="n">
-        <v>2804.75</v>
+        <v>5413</v>
       </c>
       <c r="AB45" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC45" s="30">
-        <f>IF(B15="DIV", F15,"")</f>
+        <f>IF(B13="DIV", F13,"")</f>
         <v/>
       </c>
       <c r="AD45" s="35" t="n"/>
@@ -3210,13 +3036,13 @@
         </is>
       </c>
       <c r="D46" s="26" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E46" s="27" t="n">
-        <v>490.95</v>
+        <v>485.42</v>
       </c>
       <c r="F46" s="27" t="n">
-        <v>13746.59</v>
+        <v>970.83</v>
       </c>
       <c r="G46" s="25" t="inlineStr">
         <is>
@@ -3224,61 +3050,61 @@
         </is>
       </c>
       <c r="H46" s="26" t="n">
-        <v>13.53</v>
+        <v>0.97</v>
       </c>
       <c r="I46" s="26" t="n">
-        <v>98.45999999999999</v>
+        <v>6.96</v>
       </c>
       <c r="J46" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K46" s="29">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="L46" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="M46" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
         <v/>
       </c>
       <c r="N46" s="31">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
         <v/>
       </c>
       <c r="O46" s="29">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="P46" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="Q46" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
         <v/>
       </c>
       <c r="R46" s="30">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="S46" s="32">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="T46" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
         <v/>
       </c>
       <c r="U46" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
         <v/>
       </c>
       <c r="V46" s="33">
-        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
         <v/>
       </c>
       <c r="W46" s="33" t="n">
@@ -3288,20 +3114,20 @@
         <v>45806</v>
       </c>
       <c r="Y46" s="37">
-        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
+        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/SUM(F14:I14), "")</f>
         <v/>
       </c>
       <c r="Z46" s="38" t="n">
-        <v>-2765.73</v>
+        <v>-2701.147</v>
       </c>
       <c r="AA46" s="38" t="n">
-        <v>2805</v>
+        <v>2739.5</v>
       </c>
       <c r="AB46" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC46" s="30">
-        <f>IF(B16="DIV", F16,"")</f>
+        <f>IF(B14="DIV", F14,"")</f>
         <v/>
       </c>
       <c r="AD46" s="35" t="n"/>
@@ -3336,10 +3162,10 @@
         <v>2</v>
       </c>
       <c r="E47" s="27" t="n">
-        <v>484.9</v>
+        <v>484.15</v>
       </c>
       <c r="F47" s="27" t="n">
-        <v>969.8099999999999</v>
+        <v>968.3099999999999</v>
       </c>
       <c r="G47" s="25" t="inlineStr">
         <is>
@@ -3357,51 +3183,51 @@
         <v/>
       </c>
       <c r="K47" s="29">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), L15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="L47" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="M47" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), ((E15*D15)+L15), "")</f>
         <v/>
       </c>
       <c r="N47" s="31">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV"), D15, "")</f>
         <v/>
       </c>
       <c r="O47" s="29">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), P15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="P47" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="Q47" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), ((E15*D15)+P15), "")</f>
         <v/>
       </c>
       <c r="R47" s="30">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &lt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="S47" s="32">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), T15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="T47" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), (1-Index!$F$2*2)*((J15*D15)-(E15*D15)), "")</f>
         <v/>
       </c>
       <c r="U47" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), ((E15*D15)+T15), "")</f>
         <v/>
       </c>
       <c r="V47" s="33">
-        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
+        <f>IF(AND( C15="Buy", ISBLANK(W15), B15&lt;&gt;"DIV", NOW()-A15 &gt; 365), D15, "")</f>
         <v/>
       </c>
       <c r="W47" s="33" t="n">
@@ -3411,20 +3237,20 @@
         <v>45806</v>
       </c>
       <c r="Y47" s="37">
-        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
+        <f>IF(AND( C15="Buy", W15&lt;&gt;"", AA15&lt;&gt;"", B15&lt;&gt;"DIV"), Z15/SUM(F15:I15), "")</f>
         <v/>
       </c>
       <c r="Z47" s="38" t="n">
-        <v>-5659.147</v>
+        <v>-2765.4835</v>
       </c>
       <c r="AA47" s="38" t="n">
-        <v>5739.5</v>
+        <v>2804.75</v>
       </c>
       <c r="AB47" s="39" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AC47" s="30">
-        <f>IF(B17="DIV", F17,"")</f>
+        <f>IF(B15="DIV", F15,"")</f>
         <v/>
       </c>
       <c r="AD47" s="35" t="n"/>
@@ -3456,13 +3282,13 @@
         </is>
       </c>
       <c r="D48" s="26" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E48" s="27" t="n">
-        <v>485.67</v>
+        <v>490.95</v>
       </c>
       <c r="F48" s="27" t="n">
-        <v>971.33</v>
+        <v>13746.59</v>
       </c>
       <c r="G48" s="25" t="inlineStr">
         <is>
@@ -3470,61 +3296,61 @@
         </is>
       </c>
       <c r="H48" s="26" t="n">
-        <v>0.97</v>
+        <v>13.53</v>
       </c>
       <c r="I48" s="26" t="n">
-        <v>6.96</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="J48" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K48" s="29">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), L16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="L48" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="M48" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), ((E16*D16)+L16), "")</f>
         <v/>
       </c>
       <c r="N48" s="31">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV"), D16, "")</f>
         <v/>
       </c>
       <c r="O48" s="29">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), P16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="P48" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="Q48" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), ((E16*D16)+P16), "")</f>
         <v/>
       </c>
       <c r="R48" s="30">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &lt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="S48" s="32">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), T16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="T48" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), (1-Index!$F$2*2)*((J16*D16)-(E16*D16)), "")</f>
         <v/>
       </c>
       <c r="U48" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), ((E16*D16)+T16), "")</f>
         <v/>
       </c>
       <c r="V48" s="33">
-        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
+        <f>IF(AND( C16="Buy", ISBLANK(W16), B16&lt;&gt;"DIV", NOW()-A16 &gt; 365), D16, "")</f>
         <v/>
       </c>
       <c r="W48" s="33" t="n">
@@ -3534,20 +3360,20 @@
         <v>45806</v>
       </c>
       <c r="Y48" s="37">
-        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
+        <f>IF(AND( C16="Buy", W16&lt;&gt;"", AA16&lt;&gt;"", B16&lt;&gt;"DIV"), Z16/SUM(F16:I16), "")</f>
         <v/>
       </c>
       <c r="Z48" s="38" t="n">
-        <v>-2893.6635</v>
+        <v>-2765.73</v>
       </c>
       <c r="AA48" s="38" t="n">
-        <v>2934.75</v>
+        <v>2805</v>
       </c>
       <c r="AB48" s="39" t="n">
         <v>5</v>
       </c>
       <c r="AC48" s="30">
-        <f>IF(B18="DIV", F18,"")</f>
+        <f>IF(B16="DIV", F16,"")</f>
         <v/>
       </c>
       <c r="AD48" s="35" t="n"/>
@@ -3582,10 +3408,10 @@
         <v>2</v>
       </c>
       <c r="E49" s="27" t="n">
-        <v>485.92</v>
+        <v>484.9</v>
       </c>
       <c r="F49" s="27" t="n">
-        <v>971.83</v>
+        <v>969.8099999999999</v>
       </c>
       <c r="G49" s="25" t="inlineStr">
         <is>
@@ -3596,58 +3422,58 @@
         <v>0.97</v>
       </c>
       <c r="I49" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J49" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K49" s="29">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), L17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="L49" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="M49" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), ((E17*D17)+L17), "")</f>
         <v/>
       </c>
       <c r="N49" s="31">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV"), D17, "")</f>
         <v/>
       </c>
       <c r="O49" s="29">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), P17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="P49" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="Q49" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), ((E17*D17)+P17), "")</f>
         <v/>
       </c>
       <c r="R49" s="30">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &lt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="S49" s="32">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), T17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="T49" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), (1-Index!$F$2*2)*((J17*D17)-(E17*D17)), "")</f>
         <v/>
       </c>
       <c r="U49" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), ((E17*D17)+T17), "")</f>
         <v/>
       </c>
       <c r="V49" s="33">
-        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
+        <f>IF(AND( C17="Buy", ISBLANK(W17), B17&lt;&gt;"DIV", NOW()-A17 &gt; 365), D17, "")</f>
         <v/>
       </c>
       <c r="W49" s="33" t="n">
@@ -3657,20 +3483,20 @@
         <v>45806</v>
       </c>
       <c r="Y49" s="37">
-        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
+        <f>IF(AND( C17="Buy", W17&lt;&gt;"", AA17&lt;&gt;"", B17&lt;&gt;"DIV"), Z17/SUM(F17:I17), "")</f>
         <v/>
       </c>
       <c r="Z49" s="38" t="n">
-        <v>-3061.53</v>
+        <v>-5659.147</v>
       </c>
       <c r="AA49" s="38" t="n">
-        <v>3105</v>
+        <v>5739.5</v>
       </c>
       <c r="AB49" s="39" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AC49" s="30">
-        <f>IF(B19="DIV", F19,"")</f>
+        <f>IF(B17="DIV", F17,"")</f>
         <v/>
       </c>
       <c r="AD49" s="35" t="n"/>
@@ -3705,10 +3531,10 @@
         <v>2</v>
       </c>
       <c r="E50" s="27" t="n">
-        <v>483.95</v>
+        <v>485.67</v>
       </c>
       <c r="F50" s="27" t="n">
-        <v>967.91</v>
+        <v>971.33</v>
       </c>
       <c r="G50" s="25" t="inlineStr">
         <is>
@@ -3719,58 +3545,58 @@
         <v>0.97</v>
       </c>
       <c r="I50" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J50" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K50" s="29">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), L18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="L50" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="M50" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), ((E18*D18)+L18), "")</f>
         <v/>
       </c>
       <c r="N50" s="31">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV"), D18, "")</f>
         <v/>
       </c>
       <c r="O50" s="29">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), P18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="P50" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="Q50" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), ((E18*D18)+P18), "")</f>
         <v/>
       </c>
       <c r="R50" s="30">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &lt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="S50" s="32">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), T18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="T50" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), (1-Index!$F$2*2)*((J18*D18)-(E18*D18)), "")</f>
         <v/>
       </c>
       <c r="U50" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), ((E18*D18)+T18), "")</f>
         <v/>
       </c>
       <c r="V50" s="33">
-        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
+        <f>IF(AND( C18="Buy", ISBLANK(W18), B18&lt;&gt;"DIV", NOW()-A18 &gt; 365), D18, "")</f>
         <v/>
       </c>
       <c r="W50" s="33" t="n">
@@ -3780,20 +3606,20 @@
         <v>45806</v>
       </c>
       <c r="Y50" s="37">
-        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
+        <f>IF(AND( C18="Buy", W18&lt;&gt;"", AA18&lt;&gt;"", B18&lt;&gt;"DIV"), Z18/SUM(F18:I18), "")</f>
         <v/>
       </c>
       <c r="Z50" s="38" t="n">
-        <v>-1232.4014</v>
+        <v>-2893.6635</v>
       </c>
       <c r="AA50" s="38" t="n">
-        <v>1249.9</v>
+        <v>2934.75</v>
       </c>
       <c r="AB50" s="39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC50" s="30">
-        <f>IF(B20="DIV", F20,"")</f>
+        <f>IF(B18="DIV", F18,"")</f>
         <v/>
       </c>
       <c r="AD50" s="35" t="n"/>
@@ -3828,10 +3654,10 @@
         <v>2</v>
       </c>
       <c r="E51" s="27" t="n">
-        <v>484.65</v>
+        <v>485.92</v>
       </c>
       <c r="F51" s="27" t="n">
-        <v>969.3099999999999</v>
+        <v>971.83</v>
       </c>
       <c r="G51" s="25" t="inlineStr">
         <is>
@@ -3842,58 +3668,58 @@
         <v>0.97</v>
       </c>
       <c r="I51" s="26" t="n">
-        <v>6.94</v>
+        <v>6.96</v>
       </c>
       <c r="J51" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K51" s="29">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), L19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="L51" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="M51" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), ((E19*D19)+L19), "")</f>
         <v/>
       </c>
       <c r="N51" s="31">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV"), D19, "")</f>
         <v/>
       </c>
       <c r="O51" s="29">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), P19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="P51" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="Q51" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), ((E19*D19)+P19), "")</f>
         <v/>
       </c>
       <c r="R51" s="30">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &lt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="S51" s="32">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), T19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="T51" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), (1-Index!$F$2*2)*((J19*D19)-(E19*D19)), "")</f>
         <v/>
       </c>
       <c r="U51" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), ((E19*D19)+T19), "")</f>
         <v/>
       </c>
       <c r="V51" s="33">
-        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
+        <f>IF(AND( C19="Buy", ISBLANK(W19), B19&lt;&gt;"DIV", NOW()-A19 &gt; 365), D19, "")</f>
         <v/>
       </c>
       <c r="W51" s="33" t="n">
@@ -3903,20 +3729,20 @@
         <v>45806</v>
       </c>
       <c r="Y51" s="37">
-        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
+        <f>IF(AND( C19="Buy", W19&lt;&gt;"", AA19&lt;&gt;"", B19&lt;&gt;"DIV"), Z19/SUM(F19:I19), "")</f>
         <v/>
       </c>
       <c r="Z51" s="38" t="n">
-        <v>-1842.2424</v>
+        <v>-3061.53</v>
       </c>
       <c r="AA51" s="38" t="n">
-        <v>1868.4</v>
+        <v>3105</v>
       </c>
       <c r="AB51" s="39" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AC51" s="30">
-        <f>IF(B21="DIV", F21,"")</f>
+        <f>IF(B19="DIV", F19,"")</f>
         <v/>
       </c>
       <c r="AD51" s="35" t="n"/>
@@ -3951,10 +3777,10 @@
         <v>2</v>
       </c>
       <c r="E52" s="27" t="n">
-        <v>486.17</v>
+        <v>483.95</v>
       </c>
       <c r="F52" s="27" t="n">
-        <v>972.33</v>
+        <v>967.91</v>
       </c>
       <c r="G52" s="25" t="inlineStr">
         <is>
@@ -3965,58 +3791,58 @@
         <v>0.97</v>
       </c>
       <c r="I52" s="26" t="n">
-        <v>6.96</v>
+        <v>6.94</v>
       </c>
       <c r="J52" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K52" s="29">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), L20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="L52" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="M52" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), ((E20*D20)+L20), "")</f>
         <v/>
       </c>
       <c r="N52" s="31">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV"), D20, "")</f>
         <v/>
       </c>
       <c r="O52" s="29">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), P20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="P52" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="Q52" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), ((E20*D20)+P20), "")</f>
         <v/>
       </c>
       <c r="R52" s="30">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &lt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="S52" s="32">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), T20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="T52" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), (1-Index!$F$2*2)*((J20*D20)-(E20*D20)), "")</f>
         <v/>
       </c>
       <c r="U52" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), ((E20*D20)+T20), "")</f>
         <v/>
       </c>
       <c r="V52" s="33">
-        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
+        <f>IF(AND( C20="Buy", ISBLANK(W20), B20&lt;&gt;"DIV", NOW()-A20 &gt; 365), D20, "")</f>
         <v/>
       </c>
       <c r="W52" s="33" t="n">
@@ -4026,20 +3852,20 @@
         <v>45806</v>
       </c>
       <c r="Y52" s="37">
-        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
+        <f>IF(AND( C20="Buy", W20&lt;&gt;"", AA20&lt;&gt;"", B20&lt;&gt;"DIV"), Z20/SUM(F20:I20), "")</f>
         <v/>
       </c>
       <c r="Z52" s="38" t="n">
-        <v>-648.788</v>
+        <v>-1232.4014</v>
       </c>
       <c r="AA52" s="38" t="n">
-        <v>658</v>
+        <v>1249.9</v>
       </c>
       <c r="AB52" s="39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC52" s="30">
-        <f>IF(B22="DIV", F22,"")</f>
+        <f>IF(B20="DIV", F20,"")</f>
         <v/>
       </c>
       <c r="AD52" s="35" t="n"/>
@@ -4058,7 +3884,7 @@
     </row>
     <row r="53" ht="15.75" customHeight="1" s="62">
       <c r="A53" s="36" t="n">
-        <v>45705</v>
+        <v>45712</v>
       </c>
       <c r="B53" s="25" t="inlineStr">
         <is>
@@ -4071,13 +3897,13 @@
         </is>
       </c>
       <c r="D53" s="26" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E53" s="27" t="n">
-        <v>445.69</v>
+        <v>484.65</v>
       </c>
       <c r="F53" s="27" t="n">
-        <v>8913.73</v>
+        <v>969.3099999999999</v>
       </c>
       <c r="G53" s="25" t="inlineStr">
         <is>
@@ -4085,61 +3911,61 @@
         </is>
       </c>
       <c r="H53" s="26" t="n">
-        <v>8.83</v>
+        <v>0.97</v>
       </c>
       <c r="I53" s="26" t="n">
-        <v>63.9</v>
+        <v>6.94</v>
       </c>
       <c r="J53" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K53" s="29">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), L21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="L53" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="M53" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), ((E21*D21)+L21), "")</f>
         <v/>
       </c>
       <c r="N53" s="31">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV"), D21, "")</f>
         <v/>
       </c>
       <c r="O53" s="29">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), P21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="P53" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="Q53" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), ((E21*D21)+P21), "")</f>
         <v/>
       </c>
       <c r="R53" s="30">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &lt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="S53" s="32">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), T21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="T53" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), (1-Index!$F$2*2)*((J21*D21)-(E21*D21)), "")</f>
         <v/>
       </c>
       <c r="U53" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), ((E21*D21)+T21), "")</f>
         <v/>
       </c>
       <c r="V53" s="33">
-        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
+        <f>IF(AND( C21="Buy", ISBLANK(W21), B21&lt;&gt;"DIV", NOW()-A21 &gt; 365), D21, "")</f>
         <v/>
       </c>
       <c r="W53" s="33" t="n">
@@ -4149,20 +3975,20 @@
         <v>45806</v>
       </c>
       <c r="Y53" s="37">
-        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
+        <f>IF(AND( C21="Buy", W21&lt;&gt;"", AA21&lt;&gt;"", B21&lt;&gt;"DIV"), Z21/SUM(F21:I21), "")</f>
         <v/>
       </c>
       <c r="Z53" s="38" t="n">
-        <v>-1297.4774</v>
+        <v>-1842.2424</v>
       </c>
       <c r="AA53" s="38" t="n">
-        <v>1315.9</v>
+        <v>1868.4</v>
       </c>
       <c r="AB53" s="39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC53" s="30">
-        <f>IF(B23="DIV", F23,"")</f>
+        <f>IF(B21="DIV", F21,"")</f>
         <v/>
       </c>
       <c r="AD53" s="35" t="n"/>
@@ -4181,7 +4007,7 @@
     </row>
     <row r="54" ht="15.75" customHeight="1" s="62">
       <c r="A54" s="36" t="n">
-        <v>45699</v>
+        <v>45712</v>
       </c>
       <c r="B54" s="25" t="inlineStr">
         <is>
@@ -4194,13 +4020,13 @@
         </is>
       </c>
       <c r="D54" s="26" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E54" s="27" t="n">
-        <v>509.46</v>
+        <v>486.17</v>
       </c>
       <c r="F54" s="27" t="n">
-        <v>5094.65</v>
+        <v>972.33</v>
       </c>
       <c r="G54" s="25" t="inlineStr">
         <is>
@@ -4208,61 +4034,61 @@
         </is>
       </c>
       <c r="H54" s="26" t="n">
-        <v>5.05</v>
+        <v>0.97</v>
       </c>
       <c r="I54" s="26" t="n">
-        <v>36.6</v>
+        <v>6.96</v>
       </c>
       <c r="J54" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K54" s="29">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), L22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="L54" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="M54" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), ((E22*D22)+L22), "")</f>
         <v/>
       </c>
       <c r="N54" s="31">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV"), D22, "")</f>
         <v/>
       </c>
       <c r="O54" s="29">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), P22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="P54" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="Q54" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), ((E22*D22)+P22), "")</f>
         <v/>
       </c>
       <c r="R54" s="30">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &lt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="S54" s="32">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), T22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="T54" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), (1-Index!$F$2*2)*((J22*D22)-(E22*D22)), "")</f>
         <v/>
       </c>
       <c r="U54" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), ((E22*D22)+T22), "")</f>
         <v/>
       </c>
       <c r="V54" s="33">
-        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
+        <f>IF(AND( C22="Buy", ISBLANK(W22), B22&lt;&gt;"DIV", NOW()-A22 &gt; 365), D22, "")</f>
         <v/>
       </c>
       <c r="W54" s="33" t="n">
@@ -4272,20 +4098,20 @@
         <v>45806</v>
       </c>
       <c r="Y54" s="37">
-        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
+        <f>IF(AND( C22="Buy", W22&lt;&gt;"", AA22&lt;&gt;"", B22&lt;&gt;"DIV"), Z22/SUM(F22:I22), "")</f>
         <v/>
       </c>
       <c r="Z54" s="38" t="n">
-        <v>-1295.604</v>
+        <v>-648.788</v>
       </c>
       <c r="AA54" s="38" t="n">
-        <v>1314</v>
+        <v>658</v>
       </c>
       <c r="AB54" s="39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC54" s="30">
-        <f>IF(B24="DIV", F24,"")</f>
+        <f>IF(B22="DIV", F22,"")</f>
         <v/>
       </c>
       <c r="AD54" s="35" t="n"/>
@@ -4304,7 +4130,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1" s="62">
       <c r="A55" s="36" t="n">
-        <v>45694</v>
+        <v>45705</v>
       </c>
       <c r="B55" s="25" t="inlineStr">
         <is>
@@ -4320,10 +4146,10 @@
         <v>20</v>
       </c>
       <c r="E55" s="27" t="n">
-        <v>529.3200000000001</v>
+        <v>445.69</v>
       </c>
       <c r="F55" s="27" t="n">
-        <v>10586.46</v>
+        <v>8913.73</v>
       </c>
       <c r="G55" s="25" t="inlineStr">
         <is>
@@ -4331,61 +4157,61 @@
         </is>
       </c>
       <c r="H55" s="26" t="n">
-        <v>10.47</v>
+        <v>8.83</v>
       </c>
       <c r="I55" s="26" t="n">
-        <v>75.98999999999999</v>
+        <v>63.9</v>
       </c>
       <c r="J55" s="28">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K55" s="29">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), L23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="L55" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="M55" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), ((E23*D23)+L23), "")</f>
         <v/>
       </c>
       <c r="N55" s="31">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV"), D23, "")</f>
         <v/>
       </c>
       <c r="O55" s="29">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), P23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="P55" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="Q55" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), ((E23*D23)+P23), "")</f>
         <v/>
       </c>
       <c r="R55" s="30">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &lt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="S55" s="32">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), T23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="T55" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), (1-Index!$F$2*2)*((J23*D23)-(E23*D23)), "")</f>
         <v/>
       </c>
       <c r="U55" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), ((E23*D23)+T23), "")</f>
         <v/>
       </c>
       <c r="V55" s="33">
-        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <f>IF(AND( C23="Buy", ISBLANK(W23), B23&lt;&gt;"DIV", NOW()-A23 &gt; 365), D23, "")</f>
         <v/>
       </c>
       <c r="W55" s="33" t="n">
@@ -4395,20 +4221,20 @@
         <v>45806</v>
       </c>
       <c r="Y55" s="37">
-        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <f>IF(AND( C23="Buy", W23&lt;&gt;"", AA23&lt;&gt;"", B23&lt;&gt;"DIV"), Z23/SUM(F23:I23), "")</f>
         <v/>
       </c>
       <c r="Z55" s="38" t="n">
-        <v>-5624.637</v>
+        <v>-1297.4774</v>
       </c>
       <c r="AA55" s="38" t="n">
-        <v>5704.5</v>
+        <v>1315.9</v>
       </c>
       <c r="AB55" s="39" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AC55" s="30">
-        <f>IF(B25="DIV", F25,"")</f>
+        <f>IF(B23="DIV", F23,"")</f>
         <v/>
       </c>
       <c r="AD55" s="35" t="n"/>
@@ -4426,36 +4252,250 @@
       <c r="AP55" s="40" t="n"/>
     </row>
     <row r="56" ht="15.75" customHeight="1" s="62">
-      <c r="E56" s="41" t="n"/>
-      <c r="F56" s="41" t="n"/>
-      <c r="G56" s="42" t="n"/>
-      <c r="J56" s="41" t="n"/>
-      <c r="K56" s="41" t="n"/>
-      <c r="L56" s="41" t="n"/>
-      <c r="M56" s="1" t="n"/>
-      <c r="W56" s="41" t="n"/>
-      <c r="X56" s="41" t="n"/>
-      <c r="Y56" s="41" t="n"/>
-      <c r="Z56" s="41" t="n"/>
-      <c r="AA56" s="41" t="n"/>
-      <c r="AB56" s="41" t="n"/>
-      <c r="AC56" s="41" t="n"/>
+      <c r="A56" s="36" t="n">
+        <v>45699</v>
+      </c>
+      <c r="B56" s="25" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C56" s="25" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D56" s="26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E56" s="27" t="n">
+        <v>509.46</v>
+      </c>
+      <c r="F56" s="27" t="n">
+        <v>5094.65</v>
+      </c>
+      <c r="G56" s="25" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H56" s="26" t="n">
+        <v>5.05</v>
+      </c>
+      <c r="I56" s="26" t="n">
+        <v>36.6</v>
+      </c>
+      <c r="J56" s="28">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K56" s="29">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), L24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="L56" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <v/>
+      </c>
+      <c r="M56" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), ((E24*D24)+L24), "")</f>
+        <v/>
+      </c>
+      <c r="N56" s="31">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV"), D24, "")</f>
+        <v/>
+      </c>
+      <c r="O56" s="29">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), P24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="P56" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <v/>
+      </c>
+      <c r="Q56" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), ((E24*D24)+P24), "")</f>
+        <v/>
+      </c>
+      <c r="R56" s="30">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &lt; 365), D24, "")</f>
+        <v/>
+      </c>
+      <c r="S56" s="32">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), T24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="T56" s="33">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), (1-Index!$F$2*2)*((J24*D24)-(E24*D24)), "")</f>
+        <v/>
+      </c>
+      <c r="U56" s="33">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), ((E24*D24)+T24), "")</f>
+        <v/>
+      </c>
+      <c r="V56" s="33">
+        <f>IF(AND( C24="Buy", ISBLANK(W24), B24&lt;&gt;"DIV", NOW()-A24 &gt; 365), D24, "")</f>
+        <v/>
+      </c>
+      <c r="W56" s="33" t="n">
+        <v>703.9400000000001</v>
+      </c>
+      <c r="X56" s="36" t="n">
+        <v>45806</v>
+      </c>
+      <c r="Y56" s="37">
+        <f>IF(AND( C24="Buy", W24&lt;&gt;"", AA24&lt;&gt;"", B24&lt;&gt;"DIV"), Z24/SUM(F24:I24), "")</f>
+        <v/>
+      </c>
+      <c r="Z56" s="38" t="n">
+        <v>-1295.604</v>
+      </c>
+      <c r="AA56" s="38" t="n">
+        <v>1314</v>
+      </c>
+      <c r="AB56" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC56" s="30">
+        <f>IF(B24="DIV", F24,"")</f>
+        <v/>
+      </c>
+      <c r="AD56" s="35" t="n"/>
+      <c r="AE56" s="40" t="n"/>
+      <c r="AF56" s="40" t="n"/>
+      <c r="AG56" s="40" t="n"/>
+      <c r="AH56" s="40" t="n"/>
+      <c r="AI56" s="40" t="n"/>
+      <c r="AJ56" s="40" t="n"/>
+      <c r="AK56" s="40" t="n"/>
+      <c r="AL56" s="40" t="n"/>
+      <c r="AM56" s="40" t="n"/>
+      <c r="AN56" s="40" t="n"/>
+      <c r="AO56" s="40" t="n"/>
+      <c r="AP56" s="40" t="n"/>
     </row>
     <row r="57" ht="15.75" customHeight="1" s="62">
-      <c r="E57" s="41" t="n"/>
-      <c r="F57" s="41" t="n"/>
-      <c r="G57" s="42" t="n"/>
-      <c r="J57" s="41" t="n"/>
-      <c r="K57" s="41" t="n"/>
-      <c r="L57" s="41" t="n"/>
-      <c r="M57" s="1" t="n"/>
-      <c r="W57" s="41" t="n"/>
-      <c r="X57" s="41" t="n"/>
-      <c r="Y57" s="41" t="n"/>
-      <c r="Z57" s="41" t="n"/>
-      <c r="AA57" s="41" t="n"/>
-      <c r="AB57" s="41" t="n"/>
-      <c r="AC57" s="41" t="n"/>
+      <c r="A57" s="36" t="n">
+        <v>45694</v>
+      </c>
+      <c r="B57" s="25" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C57" s="25" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D57" s="26" t="n">
+        <v>20</v>
+      </c>
+      <c r="E57" s="27" t="n">
+        <v>529.3200000000001</v>
+      </c>
+      <c r="F57" s="27" t="n">
+        <v>10586.46</v>
+      </c>
+      <c r="G57" s="25" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H57" s="26" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="I57" s="26" t="n">
+        <v>75.98999999999999</v>
+      </c>
+      <c r="J57" s="28">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K57" s="29">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), L25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="L57" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="M57" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), ((E25*D25)+L25), "")</f>
+        <v/>
+      </c>
+      <c r="N57" s="31">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV"), D25, "")</f>
+        <v/>
+      </c>
+      <c r="O57" s="29">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), P25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="P57" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="Q57" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), ((E25*D25)+P25), "")</f>
+        <v/>
+      </c>
+      <c r="R57" s="30">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &lt; 365), D25, "")</f>
+        <v/>
+      </c>
+      <c r="S57" s="32">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), T25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="T57" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), (1-Index!$F$2*2)*((J25*D25)-(E25*D25)), "")</f>
+        <v/>
+      </c>
+      <c r="U57" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), ((E25*D25)+T25), "")</f>
+        <v/>
+      </c>
+      <c r="V57" s="33">
+        <f>IF(AND( C25="Buy", ISBLANK(W25), B25&lt;&gt;"DIV", NOW()-A25 &gt; 365), D25, "")</f>
+        <v/>
+      </c>
+      <c r="W57" s="33" t="n">
+        <v>703.9400000000001</v>
+      </c>
+      <c r="X57" s="36" t="n">
+        <v>45806</v>
+      </c>
+      <c r="Y57" s="37">
+        <f>IF(AND( C25="Buy", W25&lt;&gt;"", AA25&lt;&gt;"", B25&lt;&gt;"DIV"), Z25/SUM(F25:I25), "")</f>
+        <v/>
+      </c>
+      <c r="Z57" s="38" t="n">
+        <v>-5624.637</v>
+      </c>
+      <c r="AA57" s="38" t="n">
+        <v>5704.5</v>
+      </c>
+      <c r="AB57" s="39" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC57" s="30">
+        <f>IF(B25="DIV", F25,"")</f>
+        <v/>
+      </c>
+      <c r="AD57" s="35" t="n"/>
+      <c r="AE57" s="40" t="n"/>
+      <c r="AF57" s="40" t="n"/>
+      <c r="AG57" s="40" t="n"/>
+      <c r="AH57" s="40" t="n"/>
+      <c r="AI57" s="40" t="n"/>
+      <c r="AJ57" s="40" t="n"/>
+      <c r="AK57" s="40" t="n"/>
+      <c r="AL57" s="40" t="n"/>
+      <c r="AM57" s="40" t="n"/>
+      <c r="AN57" s="40" t="n"/>
+      <c r="AO57" s="40" t="n"/>
+      <c r="AP57" s="40" t="n"/>
     </row>
     <row r="58" ht="15.75" customHeight="1" s="62">
       <c r="E58" s="41" t="n"/>
@@ -19408,6 +19448,7 @@
       <c r="J992" s="41" t="n"/>
       <c r="K992" s="41" t="n"/>
       <c r="L992" s="41" t="n"/>
+      <c r="M992" s="1" t="n"/>
       <c r="W992" s="41" t="n"/>
       <c r="X992" s="41" t="n"/>
       <c r="Y992" s="41" t="n"/>
@@ -19423,6 +19464,7 @@
       <c r="J993" s="41" t="n"/>
       <c r="K993" s="41" t="n"/>
       <c r="L993" s="41" t="n"/>
+      <c r="M993" s="1" t="n"/>
       <c r="W993" s="41" t="n"/>
       <c r="X993" s="41" t="n"/>
       <c r="Y993" s="41" t="n"/>
@@ -19655,6 +19697,36 @@
       <c r="AA1008" s="41" t="n"/>
       <c r="AB1008" s="41" t="n"/>
       <c r="AC1008" s="41" t="n"/>
+    </row>
+    <row r="1009">
+      <c r="E1009" s="41" t="n"/>
+      <c r="F1009" s="41" t="n"/>
+      <c r="G1009" s="42" t="n"/>
+      <c r="J1009" s="41" t="n"/>
+      <c r="K1009" s="41" t="n"/>
+      <c r="L1009" s="41" t="n"/>
+      <c r="W1009" s="41" t="n"/>
+      <c r="X1009" s="41" t="n"/>
+      <c r="Y1009" s="41" t="n"/>
+      <c r="Z1009" s="41" t="n"/>
+      <c r="AA1009" s="41" t="n"/>
+      <c r="AB1009" s="41" t="n"/>
+      <c r="AC1009" s="41" t="n"/>
+    </row>
+    <row r="1010">
+      <c r="E1010" s="41" t="n"/>
+      <c r="F1010" s="41" t="n"/>
+      <c r="G1010" s="42" t="n"/>
+      <c r="J1010" s="41" t="n"/>
+      <c r="K1010" s="41" t="n"/>
+      <c r="L1010" s="41" t="n"/>
+      <c r="W1010" s="41" t="n"/>
+      <c r="X1010" s="41" t="n"/>
+      <c r="Y1010" s="41" t="n"/>
+      <c r="Z1010" s="41" t="n"/>
+      <c r="AA1010" s="41" t="n"/>
+      <c r="AB1010" s="41" t="n"/>
+      <c r="AC1010" s="41" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:AO53"/>

</xml_diff>